<commit_message>
Code alternate versions of Table 3 for AX
</commit_message>
<xml_diff>
--- a/data/analysis_hh.xlsx
+++ b/data/analysis_hh.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2202" uniqueCount="1256">
   <si>
     <t>name</t>
   </si>
@@ -1274,6 +1274,2391 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t>perm</t>
+  </si>
+  <si>
+    <t>catyes</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Non-permanent Housing</t>
+  </si>
+  <si>
+    <t>Permanent Housing</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Don't Know</t>
+  </si>
+  <si>
+    <t>Neelum</t>
+  </si>
+  <si>
+    <t>Abbotabad</t>
+  </si>
+  <si>
+    <t>Bagh</t>
+  </si>
+  <si>
+    <t>Mansehra</t>
+  </si>
+  <si>
+    <t>Muzaffarabad</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>censusid</t>
+  </si>
+  <si>
+    <t>hh_assets_pca_post</t>
+  </si>
+  <si>
+    <t>hh_assets_pca_pre</t>
+  </si>
+  <si>
+    <t>hh_consumption_food</t>
+  </si>
+  <si>
+    <t>hh_consumption_nonfood</t>
+  </si>
+  <si>
+    <t>hh_death_eligible</t>
+  </si>
+  <si>
+    <t>hh_district</t>
+  </si>
+  <si>
+    <t>hh_district_1</t>
+  </si>
+  <si>
+    <t>hh_district_2</t>
+  </si>
+  <si>
+    <t>hh_district_3</t>
+  </si>
+  <si>
+    <t>hh_district_4</t>
+  </si>
+  <si>
+    <t>hh_epidist</t>
+  </si>
+  <si>
+    <t>hh_familysize</t>
+  </si>
+  <si>
+    <t>hh_fault_minimum</t>
+  </si>
+  <si>
+    <t>hh_faultdist</t>
+  </si>
+  <si>
+    <t>hh_housing_amount</t>
+  </si>
+  <si>
+    <t>hh_housing_eligible</t>
+  </si>
+  <si>
+    <t>hh_housing_mSec16_q1_trench1</t>
+  </si>
+  <si>
+    <t>hh_injury_eligible</t>
+  </si>
+  <si>
+    <t>hh_lcgs_eligible</t>
+  </si>
+  <si>
+    <t>hh_slope</t>
+  </si>
+  <si>
+    <t>hh_stats_electricity_post</t>
+  </si>
+  <si>
+    <t>hh_stats_electricity_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_govtschool_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_logdistrict_post</t>
+  </si>
+  <si>
+    <t>hh_stats_loggschool_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logmarket_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logmedical_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logprischool_post</t>
+  </si>
+  <si>
+    <t>hh_stats_market_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_medical_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_privateschool_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_water_dist_pre</t>
+  </si>
+  <si>
+    <t>village_code</t>
+  </si>
+  <si>
+    <t>hh_aid_any_1</t>
+  </si>
+  <si>
+    <t>hh_aid_any_2</t>
+  </si>
+  <si>
+    <t>hh_aid_any_3</t>
+  </si>
+  <si>
+    <t>hh_aid_any_4</t>
+  </si>
+  <si>
+    <t>hh_aid_any_5</t>
+  </si>
+  <si>
+    <t>hh_aid_any_6</t>
+  </si>
+  <si>
+    <t>hh_elevation_binary</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_1</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_2</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_4</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_5</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_6</t>
+  </si>
+  <si>
+    <t>hh_far_from_quake</t>
+  </si>
+  <si>
+    <t>hh_perm_house_pre</t>
+  </si>
+  <si>
+    <t>hh_perm_house_post</t>
+  </si>
+  <si>
+    <t>hh_aid_total</t>
+  </si>
+  <si>
+    <t>hh_dead</t>
+  </si>
+  <si>
+    <t>hh_assets_1_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_2_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_3_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_4_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_5_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_6_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_7_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_8_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_9_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_10_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_11_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_12_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_13_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_14_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_15_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_16_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_17_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_18_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_19_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_20_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_21_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_22_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_23_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_24_pre</t>
+  </si>
+  <si>
+    <t>hh_water_inhouse_pre</t>
+  </si>
+  <si>
+    <t>hh_water_inhouse_post</t>
+  </si>
+  <si>
+    <t>hh_infra_index_post</t>
+  </si>
+  <si>
+    <t>tag_uc</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Census ID</t>
+  </si>
+  <si>
+    <t>Asset Index (PCA) (Post-Quake)</t>
+  </si>
+  <si>
+    <t>Asset Index (PCA) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Total Annual Food Expenditure</t>
+  </si>
+  <si>
+    <t>Total Annual Nonfood Expenditure</t>
+  </si>
+  <si>
+    <t>Eligible for death compensation?</t>
+  </si>
+  <si>
+    <t>District Code</t>
+  </si>
+  <si>
+    <t>District Abbottabad</t>
+  </si>
+  <si>
+    <t>District Bagh</t>
+  </si>
+  <si>
+    <t>District Mansehra</t>
+  </si>
+  <si>
+    <t>District Muzaffarabad</t>
+  </si>
+  <si>
+    <t>Distance to Epicenter (km)</t>
+  </si>
+  <si>
+    <t>Family Size</t>
+  </si>
+  <si>
+    <t>Closest Faultline (km)</t>
+  </si>
+  <si>
+    <t>Distance to Faultline (km)</t>
+  </si>
+  <si>
+    <t>Amount received from housing compensation</t>
+  </si>
+  <si>
+    <t>Eligible for housing compensation?</t>
+  </si>
+  <si>
+    <t>Did any member receive 1st trench of 25,000 rupee grant immediately following EQ</t>
+  </si>
+  <si>
+    <t>Eligible for injury compensation?</t>
+  </si>
+  <si>
+    <t>Eligible for lcgs compensation?</t>
+  </si>
+  <si>
+    <t>Mean Slope of UC</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Gov't School (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Log Dist to Distr Office (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Gov't School (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Market (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Medical (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Private School (min)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Market (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Medical Facility (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Private School (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Distance to Water (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Village Code</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Financial</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Health and Medical</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Shelter</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Food</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Supplies</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Liaison with other organizations</t>
+  </si>
+  <si>
+    <t>Above Median Elevation</t>
+  </si>
+  <si>
+    <t>Distance to Water (km)</t>
+  </si>
+  <si>
+    <t>Distance to Health Clinic (km)</t>
+  </si>
+  <si>
+    <t>Distance to Boys School (km)</t>
+  </si>
+  <si>
+    <t>Distance to Girls School (km)</t>
+  </si>
+  <si>
+    <t>Distance to Private School (km)</t>
+  </si>
+  <si>
+    <t>Far from Fault (&gt;20km)</t>
+  </si>
+  <si>
+    <t>Permanent House (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Total Reported Aid Compensation</t>
+  </si>
+  <si>
+    <t>Number Dead in Earthquake</t>
+  </si>
+  <si>
+    <t>Beds/Charpais</t>
+  </si>
+  <si>
+    <t>Tables</t>
+  </si>
+  <si>
+    <t>Chairs</t>
+  </si>
+  <si>
+    <t>Fans (Ceiling/Table/Pedestal/Exhaust)</t>
+  </si>
+  <si>
+    <t>Sewing machine</t>
+  </si>
+  <si>
+    <t>Books</t>
+  </si>
+  <si>
+    <t>Refrigerator</t>
+  </si>
+  <si>
+    <t>Radio/Cassette recorder/CD Player</t>
+  </si>
+  <si>
+    <t>Television</t>
+  </si>
+  <si>
+    <t>VCR/VCD</t>
+  </si>
+  <si>
+    <t>Watches</t>
+  </si>
+  <si>
+    <t>Guns</t>
+  </si>
+  <si>
+    <t>Plough</t>
+  </si>
+  <si>
+    <t>Tractor</t>
+  </si>
+  <si>
+    <t>Tube well/Hand pump</t>
+  </si>
+  <si>
+    <t>Other Agricultural Machinery</t>
+  </si>
+  <si>
+    <t>Other Agricultural Hand-Tools/Saw</t>
+  </si>
+  <si>
+    <t>Motorcycle/Scooter</t>
+  </si>
+  <si>
+    <t>Car/Taxi/Vehicle</t>
+  </si>
+  <si>
+    <t>Bicycle</t>
+  </si>
+  <si>
+    <t>Cattle</t>
+  </si>
+  <si>
+    <t>Goats</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Mobile Phone</t>
+  </si>
+  <si>
+    <t>Water In House (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Water In House (Post-Quake)</t>
+  </si>
+  <si>
+    <t>Household Infrastructure Index</t>
+  </si>
+  <si>
+    <t>Union Council Tag</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>choices</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>catyes</t>
+  </si>
+  <si>
+    <t>hh_elevation_binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>perm</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>dead_l</t>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t>perm</t>
+  </si>
+  <si>
+    <t>catyes</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Non-permanent Housing</t>
+  </si>
+  <si>
+    <t>Permanent Housing</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Don't Know</t>
+  </si>
+  <si>
+    <t>Neelum</t>
+  </si>
+  <si>
+    <t>Abbotabad</t>
+  </si>
+  <si>
+    <t>Bagh</t>
+  </si>
+  <si>
+    <t>Mansehra</t>
+  </si>
+  <si>
+    <t>Muzaffarabad</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>censusid</t>
+  </si>
+  <si>
+    <t>hh_assets_pca_post</t>
+  </si>
+  <si>
+    <t>hh_assets_pca_pre</t>
+  </si>
+  <si>
+    <t>hh_consumption_food</t>
+  </si>
+  <si>
+    <t>hh_consumption_nonfood</t>
+  </si>
+  <si>
+    <t>hh_death_eligible</t>
+  </si>
+  <si>
+    <t>hh_district</t>
+  </si>
+  <si>
+    <t>hh_district_1</t>
+  </si>
+  <si>
+    <t>hh_district_2</t>
+  </si>
+  <si>
+    <t>hh_district_3</t>
+  </si>
+  <si>
+    <t>hh_district_4</t>
+  </si>
+  <si>
+    <t>hh_epidist</t>
+  </si>
+  <si>
+    <t>hh_familysize</t>
+  </si>
+  <si>
+    <t>hh_fault_minimum</t>
+  </si>
+  <si>
+    <t>hh_faultdist</t>
+  </si>
+  <si>
+    <t>hh_housing_amount</t>
+  </si>
+  <si>
+    <t>hh_housing_eligible</t>
+  </si>
+  <si>
+    <t>hh_housing_mSec16_q1_trench1</t>
+  </si>
+  <si>
+    <t>hh_injury_eligible</t>
+  </si>
+  <si>
+    <t>hh_lcgs_eligible</t>
+  </si>
+  <si>
+    <t>hh_slope</t>
+  </si>
+  <si>
+    <t>hh_stats_electricity_post</t>
+  </si>
+  <si>
+    <t>hh_stats_electricity_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_govtschool_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_logdistrict_post</t>
+  </si>
+  <si>
+    <t>hh_stats_loggschool_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logmarket_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logmedical_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logprischool_post</t>
+  </si>
+  <si>
+    <t>hh_stats_market_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_medical_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_privateschool_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_water_dist_pre</t>
+  </si>
+  <si>
+    <t>village_code</t>
+  </si>
+  <si>
+    <t>hh_aid_any_1</t>
+  </si>
+  <si>
+    <t>hh_aid_any_2</t>
+  </si>
+  <si>
+    <t>hh_aid_any_3</t>
+  </si>
+  <si>
+    <t>hh_aid_any_4</t>
+  </si>
+  <si>
+    <t>hh_aid_any_5</t>
+  </si>
+  <si>
+    <t>hh_aid_any_6</t>
+  </si>
+  <si>
+    <t>hh_elevation_binary</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_1</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_2</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_4</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_5</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_6</t>
+  </si>
+  <si>
+    <t>hh_far_from_quake</t>
+  </si>
+  <si>
+    <t>hh_perm_house_pre</t>
+  </si>
+  <si>
+    <t>hh_perm_house_post</t>
+  </si>
+  <si>
+    <t>hh_aid_total</t>
+  </si>
+  <si>
+    <t>hh_dead</t>
+  </si>
+  <si>
+    <t>hh_assets_1_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_2_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_3_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_4_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_5_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_6_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_7_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_8_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_9_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_10_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_11_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_12_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_13_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_14_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_15_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_16_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_17_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_18_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_19_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_20_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_21_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_22_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_23_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_24_pre</t>
+  </si>
+  <si>
+    <t>hh_water_inhouse_pre</t>
+  </si>
+  <si>
+    <t>hh_water_inhouse_post</t>
+  </si>
+  <si>
+    <t>hh_infra_index_post</t>
+  </si>
+  <si>
+    <t>tag_uc</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Census ID</t>
+  </si>
+  <si>
+    <t>Asset Index (PCA) (Post-Quake)</t>
+  </si>
+  <si>
+    <t>Asset Index (PCA) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Total Annual Food Expenditure</t>
+  </si>
+  <si>
+    <t>Total Annual Nonfood Expenditure</t>
+  </si>
+  <si>
+    <t>Eligible for death compensation?</t>
+  </si>
+  <si>
+    <t>District Code</t>
+  </si>
+  <si>
+    <t>District Abbottabad</t>
+  </si>
+  <si>
+    <t>District Bagh</t>
+  </si>
+  <si>
+    <t>District Mansehra</t>
+  </si>
+  <si>
+    <t>District Muzaffarabad</t>
+  </si>
+  <si>
+    <t>Distance to Epicenter (km)</t>
+  </si>
+  <si>
+    <t>Family Size</t>
+  </si>
+  <si>
+    <t>Closest Faultline (km)</t>
+  </si>
+  <si>
+    <t>Distance to Faultline (km)</t>
+  </si>
+  <si>
+    <t>Amount received from housing compensation</t>
+  </si>
+  <si>
+    <t>Eligible for housing compensation?</t>
+  </si>
+  <si>
+    <t>Did any member receive 1st trench of 25,000 rupee grant immediately following EQ</t>
+  </si>
+  <si>
+    <t>Eligible for injury compensation?</t>
+  </si>
+  <si>
+    <t>Eligible for lcgs compensation?</t>
+  </si>
+  <si>
+    <t>Mean Slope of UC</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Gov't School (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Log Dist to Distr Office (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Gov't School (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Market (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Medical (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Private School (min)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Market (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Medical Facility (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Private School (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Distance to Water (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Village Code</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Financial</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Health and Medical</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Shelter</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Food</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Supplies</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Liaison with other organizations</t>
+  </si>
+  <si>
+    <t>Above Median Elevation</t>
+  </si>
+  <si>
+    <t>Distance to Water (km)</t>
+  </si>
+  <si>
+    <t>Distance to Health Clinic (km)</t>
+  </si>
+  <si>
+    <t>Distance to Boys School (km)</t>
+  </si>
+  <si>
+    <t>Distance to Girls School (km)</t>
+  </si>
+  <si>
+    <t>Distance to Private School (km)</t>
+  </si>
+  <si>
+    <t>Far from Fault (&gt;20km)</t>
+  </si>
+  <si>
+    <t>Permanent House (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Total Reported Aid Compensation</t>
+  </si>
+  <si>
+    <t>Number Dead in Earthquake</t>
+  </si>
+  <si>
+    <t>Beds/Charpais</t>
+  </si>
+  <si>
+    <t>Tables</t>
+  </si>
+  <si>
+    <t>Chairs</t>
+  </si>
+  <si>
+    <t>Fans (Ceiling/Table/Pedestal/Exhaust)</t>
+  </si>
+  <si>
+    <t>Sewing machine</t>
+  </si>
+  <si>
+    <t>Books</t>
+  </si>
+  <si>
+    <t>Refrigerator</t>
+  </si>
+  <si>
+    <t>Radio/Cassette recorder/CD Player</t>
+  </si>
+  <si>
+    <t>Television</t>
+  </si>
+  <si>
+    <t>VCR/VCD</t>
+  </si>
+  <si>
+    <t>Watches</t>
+  </si>
+  <si>
+    <t>Guns</t>
+  </si>
+  <si>
+    <t>Plough</t>
+  </si>
+  <si>
+    <t>Tractor</t>
+  </si>
+  <si>
+    <t>Tube well/Hand pump</t>
+  </si>
+  <si>
+    <t>Other Agricultural Machinery</t>
+  </si>
+  <si>
+    <t>Other Agricultural Hand-Tools/Saw</t>
+  </si>
+  <si>
+    <t>Motorcycle/Scooter</t>
+  </si>
+  <si>
+    <t>Car/Taxi/Vehicle</t>
+  </si>
+  <si>
+    <t>Bicycle</t>
+  </si>
+  <si>
+    <t>Cattle</t>
+  </si>
+  <si>
+    <t>Goats</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Mobile Phone</t>
+  </si>
+  <si>
+    <t>Water In House (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Water In House (Post-Quake)</t>
+  </si>
+  <si>
+    <t>Household Infrastructure Index</t>
+  </si>
+  <si>
+    <t>Union Council Tag</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>choices</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>catyes</t>
+  </si>
+  <si>
+    <t>hh_elevation_binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>perm</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>dead_l</t>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t>perm</t>
+  </si>
+  <si>
+    <t>catyes</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Non-permanent Housing</t>
+  </si>
+  <si>
+    <t>Permanent Housing</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Don't Know</t>
+  </si>
+  <si>
+    <t>Neelum</t>
+  </si>
+  <si>
+    <t>Abbotabad</t>
+  </si>
+  <si>
+    <t>Bagh</t>
+  </si>
+  <si>
+    <t>Mansehra</t>
+  </si>
+  <si>
+    <t>Muzaffarabad</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>censusid</t>
+  </si>
+  <si>
+    <t>hh_assets_pca_post</t>
+  </si>
+  <si>
+    <t>hh_assets_pca_pre</t>
+  </si>
+  <si>
+    <t>hh_consumption_food</t>
+  </si>
+  <si>
+    <t>hh_consumption_nonfood</t>
+  </si>
+  <si>
+    <t>hh_death_eligible</t>
+  </si>
+  <si>
+    <t>hh_district</t>
+  </si>
+  <si>
+    <t>hh_district_1</t>
+  </si>
+  <si>
+    <t>hh_district_2</t>
+  </si>
+  <si>
+    <t>hh_district_3</t>
+  </si>
+  <si>
+    <t>hh_district_4</t>
+  </si>
+  <si>
+    <t>hh_epidist</t>
+  </si>
+  <si>
+    <t>hh_familysize</t>
+  </si>
+  <si>
+    <t>hh_fault_minimum</t>
+  </si>
+  <si>
+    <t>hh_faultdist</t>
+  </si>
+  <si>
+    <t>hh_housing_amount</t>
+  </si>
+  <si>
+    <t>hh_housing_eligible</t>
+  </si>
+  <si>
+    <t>hh_housing_mSec16_q1_trench1</t>
+  </si>
+  <si>
+    <t>hh_injury_eligible</t>
+  </si>
+  <si>
+    <t>hh_lcgs_eligible</t>
+  </si>
+  <si>
+    <t>hh_slope</t>
+  </si>
+  <si>
+    <t>hh_stats_electricity_post</t>
+  </si>
+  <si>
+    <t>hh_stats_electricity_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_govtschool_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_logdistrict_post</t>
+  </si>
+  <si>
+    <t>hh_stats_loggschool_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logmarket_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logmedical_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logprischool_post</t>
+  </si>
+  <si>
+    <t>hh_stats_market_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_medical_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_privateschool_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_water_dist_pre</t>
+  </si>
+  <si>
+    <t>village_code</t>
+  </si>
+  <si>
+    <t>hh_aid_any_1</t>
+  </si>
+  <si>
+    <t>hh_aid_any_2</t>
+  </si>
+  <si>
+    <t>hh_aid_any_3</t>
+  </si>
+  <si>
+    <t>hh_aid_any_4</t>
+  </si>
+  <si>
+    <t>hh_aid_any_5</t>
+  </si>
+  <si>
+    <t>hh_aid_any_6</t>
+  </si>
+  <si>
+    <t>hh_elevation_binary</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_1</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_2</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_4</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_5</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_6</t>
+  </si>
+  <si>
+    <t>hh_far_from_quake</t>
+  </si>
+  <si>
+    <t>hh_perm_house_pre</t>
+  </si>
+  <si>
+    <t>hh_perm_house_post</t>
+  </si>
+  <si>
+    <t>hh_aid_total</t>
+  </si>
+  <si>
+    <t>hh_dead</t>
+  </si>
+  <si>
+    <t>hh_assets_1_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_2_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_3_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_4_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_5_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_6_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_7_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_8_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_9_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_10_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_11_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_12_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_13_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_14_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_15_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_16_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_17_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_18_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_19_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_20_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_21_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_22_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_23_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_24_pre</t>
+  </si>
+  <si>
+    <t>hh_water_inhouse_pre</t>
+  </si>
+  <si>
+    <t>hh_water_inhouse_post</t>
+  </si>
+  <si>
+    <t>hh_infra_index_post</t>
+  </si>
+  <si>
+    <t>tag_uc</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Census ID</t>
+  </si>
+  <si>
+    <t>Asset Index (PCA) (Post-Quake)</t>
+  </si>
+  <si>
+    <t>Asset Index (PCA) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Total Annual Food Expenditure</t>
+  </si>
+  <si>
+    <t>Total Annual Nonfood Expenditure</t>
+  </si>
+  <si>
+    <t>Eligible for death compensation?</t>
+  </si>
+  <si>
+    <t>District Code</t>
+  </si>
+  <si>
+    <t>District Abbottabad</t>
+  </si>
+  <si>
+    <t>District Bagh</t>
+  </si>
+  <si>
+    <t>District Mansehra</t>
+  </si>
+  <si>
+    <t>District Muzaffarabad</t>
+  </si>
+  <si>
+    <t>Distance to Epicenter (km)</t>
+  </si>
+  <si>
+    <t>Family Size</t>
+  </si>
+  <si>
+    <t>Closest Faultline (km)</t>
+  </si>
+  <si>
+    <t>Distance to Faultline (km)</t>
+  </si>
+  <si>
+    <t>Amount received from housing compensation</t>
+  </si>
+  <si>
+    <t>Eligible for housing compensation?</t>
+  </si>
+  <si>
+    <t>Did any member receive 1st trench of 25,000 rupee grant immediately following EQ</t>
+  </si>
+  <si>
+    <t>Eligible for injury compensation?</t>
+  </si>
+  <si>
+    <t>Eligible for lcgs compensation?</t>
+  </si>
+  <si>
+    <t>Mean Slope of UC</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Gov't School (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Log Dist to Distr Office (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Gov't School (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Market (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Medical (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Private School (min)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Market (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Medical Facility (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Private School (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Distance to Water (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Village Code</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Financial</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Health and Medical</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Shelter</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Food</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Supplies</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Liaison with other organizations</t>
+  </si>
+  <si>
+    <t>Above Median Elevation</t>
+  </si>
+  <si>
+    <t>Distance to Water (km)</t>
+  </si>
+  <si>
+    <t>Distance to Health Clinic (km)</t>
+  </si>
+  <si>
+    <t>Distance to Boys School (km)</t>
+  </si>
+  <si>
+    <t>Distance to Girls School (km)</t>
+  </si>
+  <si>
+    <t>Distance to Private School (km)</t>
+  </si>
+  <si>
+    <t>Far from Fault (&gt;20km)</t>
+  </si>
+  <si>
+    <t>Permanent House (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Total Reported Aid Compensation</t>
+  </si>
+  <si>
+    <t>Number Dead in Earthquake</t>
+  </si>
+  <si>
+    <t>Beds/Charpais</t>
+  </si>
+  <si>
+    <t>Tables</t>
+  </si>
+  <si>
+    <t>Chairs</t>
+  </si>
+  <si>
+    <t>Fans (Ceiling/Table/Pedestal/Exhaust)</t>
+  </si>
+  <si>
+    <t>Sewing machine</t>
+  </si>
+  <si>
+    <t>Books</t>
+  </si>
+  <si>
+    <t>Refrigerator</t>
+  </si>
+  <si>
+    <t>Radio/Cassette recorder/CD Player</t>
+  </si>
+  <si>
+    <t>Television</t>
+  </si>
+  <si>
+    <t>VCR/VCD</t>
+  </si>
+  <si>
+    <t>Watches</t>
+  </si>
+  <si>
+    <t>Guns</t>
+  </si>
+  <si>
+    <t>Plough</t>
+  </si>
+  <si>
+    <t>Tractor</t>
+  </si>
+  <si>
+    <t>Tube well/Hand pump</t>
+  </si>
+  <si>
+    <t>Other Agricultural Machinery</t>
+  </si>
+  <si>
+    <t>Other Agricultural Hand-Tools/Saw</t>
+  </si>
+  <si>
+    <t>Motorcycle/Scooter</t>
+  </si>
+  <si>
+    <t>Car/Taxi/Vehicle</t>
+  </si>
+  <si>
+    <t>Bicycle</t>
+  </si>
+  <si>
+    <t>Cattle</t>
+  </si>
+  <si>
+    <t>Goats</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Mobile Phone</t>
+  </si>
+  <si>
+    <t>Water In House (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Water In House (Post-Quake)</t>
+  </si>
+  <si>
+    <t>Household Infrastructure Index</t>
+  </si>
+  <si>
+    <t>Union Council Tag</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>choices</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>catyes</t>
+  </si>
+  <si>
+    <t>hh_elevation_binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>perm</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>dead_l</t>
   </si>
   <si>
     <t>yesno</t>
@@ -1440,1141 +3825,1127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D80"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>191</v>
+        <v>991</v>
       </c>
       <c r="B1" t="s">
-        <v>272</v>
+        <v>1071</v>
       </c>
       <c r="C1" t="s">
-        <v>351</v>
+        <v>1149</v>
       </c>
       <c r="D1" t="s">
-        <v>376</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>192</v>
+        <v>992</v>
       </c>
       <c r="B2" t="s">
-        <v>273</v>
+        <v>1072</v>
       </c>
       <c r="C2" t="s">
-        <v>352</v>
+        <v>1150</v>
       </c>
       <c r="D2" t="s">
-        <v>377</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>993</v>
       </c>
       <c r="B3" t="s">
-        <v>274</v>
+        <v>1073</v>
       </c>
       <c r="C3" t="s">
-        <v>353</v>
+        <v>1151</v>
       </c>
       <c r="D3" t="s">
-        <v>378</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>194</v>
+        <v>994</v>
       </c>
       <c r="B4" t="s">
-        <v>275</v>
+        <v>1074</v>
       </c>
       <c r="C4" t="s">
-        <v>353</v>
+        <v>1151</v>
       </c>
       <c r="D4" t="s">
-        <v>379</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>195</v>
+        <v>995</v>
       </c>
       <c r="B5" t="s">
-        <v>276</v>
+        <v>1075</v>
       </c>
       <c r="C5" t="s">
-        <v>353</v>
+        <v>1151</v>
       </c>
       <c r="D5" t="s">
-        <v>380</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>996</v>
       </c>
       <c r="B6" t="s">
-        <v>277</v>
+        <v>1076</v>
       </c>
       <c r="C6" t="s">
-        <v>353</v>
+        <v>1151</v>
       </c>
       <c r="D6" t="s">
-        <v>381</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>197</v>
+        <v>997</v>
       </c>
       <c r="B7" t="s">
-        <v>278</v>
+        <v>1077</v>
       </c>
       <c r="C7" t="s">
-        <v>354</v>
+        <v>1152</v>
       </c>
       <c r="D7" t="s">
-        <v>382</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>198</v>
+        <v>998</v>
       </c>
       <c r="B8" t="s">
-        <v>279</v>
+        <v>1078</v>
       </c>
       <c r="C8" t="s">
-        <v>354</v>
+        <v>1152</v>
       </c>
       <c r="D8" t="s">
-        <v>383</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>199</v>
+        <v>999</v>
       </c>
       <c r="B9" t="s">
-        <v>280</v>
+        <v>1079</v>
       </c>
       <c r="C9" t="s">
-        <v>354</v>
+        <v>1152</v>
       </c>
       <c r="D9" t="s">
-        <v>384</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="B10" t="s">
-        <v>281</v>
+        <v>1080</v>
       </c>
       <c r="C10" t="s">
-        <v>354</v>
+        <v>1152</v>
       </c>
       <c r="D10" t="s">
-        <v>385</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>201</v>
+        <v>1001</v>
       </c>
       <c r="B11" t="s">
-        <v>282</v>
+        <v>1081</v>
       </c>
       <c r="C11" t="s">
-        <v>354</v>
+        <v>1152</v>
       </c>
       <c r="D11" t="s">
-        <v>386</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>202</v>
+        <v>1002</v>
       </c>
       <c r="B12" t="s">
-        <v>283</v>
+        <v>1082</v>
       </c>
       <c r="C12" t="s">
-        <v>354</v>
+        <v>1152</v>
       </c>
       <c r="D12" t="s">
-        <v>387</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>203</v>
+        <v>1003</v>
       </c>
       <c r="B13" t="s">
-        <v>284</v>
+        <v>1083</v>
       </c>
       <c r="C13" t="s">
-        <v>355</v>
+        <v>1153</v>
       </c>
       <c r="D13" t="s">
-        <v>388</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>204</v>
+        <v>1004</v>
       </c>
       <c r="B14" t="s">
-        <v>285</v>
+        <v>1084</v>
       </c>
       <c r="C14" t="s">
-        <v>356</v>
+        <v>1154</v>
       </c>
       <c r="D14" t="s">
-        <v>389</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>205</v>
+        <v>1005</v>
       </c>
       <c r="B15" t="s">
-        <v>286</v>
+        <v>1085</v>
       </c>
       <c r="C15" t="s">
-        <v>357</v>
+        <v>1155</v>
       </c>
       <c r="D15" t="s">
-        <v>390</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>206</v>
+        <v>1006</v>
       </c>
       <c r="B16" t="s">
-        <v>287</v>
+        <v>1086</v>
       </c>
       <c r="C16" t="s">
-        <v>357</v>
+        <v>1155</v>
       </c>
       <c r="D16" t="s">
-        <v>391</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>207</v>
+        <v>1007</v>
       </c>
       <c r="B17" t="s">
-        <v>288</v>
+        <v>1087</v>
       </c>
       <c r="C17" t="s">
-        <v>358</v>
+        <v>1156</v>
       </c>
       <c r="D17" t="s">
-        <v>392</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>208</v>
+        <v>1008</v>
       </c>
       <c r="B18" t="s">
-        <v>289</v>
+        <v>1088</v>
       </c>
       <c r="C18" t="s">
-        <v>359</v>
+        <v>1157</v>
       </c>
       <c r="D18" t="s">
-        <v>393</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>209</v>
+        <v>1009</v>
       </c>
       <c r="B19" t="s">
-        <v>290</v>
+        <v>1089</v>
       </c>
       <c r="C19" t="s">
-        <v>359</v>
+        <v>1157</v>
       </c>
       <c r="D19" t="s">
-        <v>393</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>210</v>
+        <v>1010</v>
       </c>
       <c r="B20" t="s">
-        <v>291</v>
+        <v>1090</v>
       </c>
       <c r="C20" t="s">
-        <v>359</v>
+        <v>1157</v>
       </c>
       <c r="D20" t="s">
-        <v>393</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>211</v>
+        <v>1011</v>
       </c>
       <c r="B21" t="s">
-        <v>292</v>
+        <v>1091</v>
       </c>
       <c r="C21" t="s">
-        <v>359</v>
+        <v>1157</v>
       </c>
       <c r="D21" t="s">
-        <v>393</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>212</v>
+        <v>1012</v>
       </c>
       <c r="B22" t="s">
-        <v>293</v>
+        <v>1092</v>
       </c>
       <c r="C22" t="s">
-        <v>360</v>
+        <v>1158</v>
       </c>
       <c r="D22" t="s">
-        <v>394</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>213</v>
+        <v>1013</v>
       </c>
       <c r="B23" t="s">
-        <v>294</v>
+        <v>1093</v>
       </c>
       <c r="C23" t="s">
-        <v>361</v>
+        <v>1159</v>
       </c>
       <c r="D23" t="s">
-        <v>395</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>214</v>
+        <v>1014</v>
       </c>
       <c r="B24" t="s">
-        <v>294</v>
+        <v>1093</v>
       </c>
       <c r="C24" t="s">
-        <v>361</v>
+        <v>1159</v>
       </c>
       <c r="D24" t="s">
-        <v>395</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>215</v>
+        <v>1015</v>
       </c>
       <c r="B25" t="s">
-        <v>295</v>
+        <v>1094</v>
       </c>
       <c r="C25" t="s">
-        <v>362</v>
+        <v>1160</v>
       </c>
       <c r="D25" t="s">
-        <v>396</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>216</v>
+        <v>1016</v>
       </c>
       <c r="B26" t="s">
-        <v>296</v>
+        <v>1095</v>
       </c>
       <c r="C26" t="s">
-        <v>363</v>
+        <v>1161</v>
       </c>
       <c r="D26" t="s">
-        <v>397</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>217</v>
+        <v>1017</v>
       </c>
       <c r="B27" t="s">
-        <v>297</v>
+        <v>1096</v>
       </c>
       <c r="C27" t="s">
-        <v>363</v>
+        <v>1161</v>
       </c>
       <c r="D27" t="s">
-        <v>398</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>218</v>
+        <v>1018</v>
       </c>
       <c r="B28" t="s">
-        <v>298</v>
+        <v>1097</v>
       </c>
       <c r="C28" t="s">
-        <v>363</v>
+        <v>1161</v>
       </c>
       <c r="D28" t="s">
-        <v>399</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>219</v>
+        <v>1019</v>
       </c>
       <c r="B29" t="s">
-        <v>299</v>
+        <v>1098</v>
       </c>
       <c r="C29" t="s">
-        <v>363</v>
+        <v>1161</v>
       </c>
       <c r="D29" t="s">
-        <v>400</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>220</v>
+        <v>1020</v>
       </c>
       <c r="B30" t="s">
-        <v>300</v>
+        <v>1099</v>
       </c>
       <c r="C30" t="s">
-        <v>363</v>
+        <v>1161</v>
       </c>
       <c r="D30" t="s">
-        <v>401</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>221</v>
+        <v>1021</v>
       </c>
       <c r="B31" t="s">
-        <v>301</v>
+        <v>1100</v>
       </c>
       <c r="C31" t="s">
-        <v>364</v>
+        <v>1162</v>
       </c>
       <c r="D31" t="s">
-        <v>402</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>222</v>
+        <v>1022</v>
       </c>
       <c r="B32" t="s">
-        <v>302</v>
+        <v>1101</v>
       </c>
       <c r="C32" t="s">
-        <v>364</v>
+        <v>1162</v>
       </c>
       <c r="D32" t="s">
-        <v>403</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>223</v>
+        <v>1023</v>
       </c>
       <c r="B33" t="s">
-        <v>303</v>
+        <v>1102</v>
       </c>
       <c r="C33" t="s">
-        <v>364</v>
+        <v>1162</v>
       </c>
       <c r="D33" t="s">
-        <v>404</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>224</v>
+        <v>1024</v>
       </c>
       <c r="B34" t="s">
-        <v>304</v>
+        <v>1103</v>
       </c>
       <c r="C34" t="s">
-        <v>365</v>
+        <v>1163</v>
       </c>
       <c r="D34" t="s">
-        <v>405</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>225</v>
+        <v>1025</v>
       </c>
       <c r="B35" t="s">
-        <v>305</v>
+        <v>1104</v>
       </c>
       <c r="C35" t="s">
-        <v>366</v>
+        <v>1164</v>
       </c>
       <c r="D35" t="s">
-        <v>406</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>226</v>
+        <v>1026</v>
       </c>
       <c r="B36" t="s">
-        <v>306</v>
+        <v>1105</v>
       </c>
       <c r="C36" t="s">
-        <v>367</v>
+        <v>1165</v>
       </c>
       <c r="D36" t="s">
-        <v>407</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>227</v>
+        <v>1027</v>
       </c>
       <c r="B37" t="s">
-        <v>307</v>
+        <v>1106</v>
       </c>
       <c r="C37" t="s">
-        <v>367</v>
+        <v>1165</v>
       </c>
       <c r="D37" t="s">
-        <v>407</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>228</v>
+        <v>1028</v>
       </c>
       <c r="B38" t="s">
-        <v>308</v>
+        <v>1107</v>
       </c>
       <c r="C38" t="s">
-        <v>367</v>
+        <v>1165</v>
       </c>
       <c r="D38" t="s">
-        <v>407</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>229</v>
+        <v>1029</v>
       </c>
       <c r="B39" t="s">
-        <v>309</v>
+        <v>1108</v>
       </c>
       <c r="C39" t="s">
-        <v>367</v>
+        <v>1165</v>
       </c>
       <c r="D39" t="s">
-        <v>407</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>230</v>
+        <v>1030</v>
       </c>
       <c r="B40" t="s">
-        <v>310</v>
+        <v>1109</v>
       </c>
       <c r="C40" t="s">
-        <v>367</v>
+        <v>1165</v>
       </c>
       <c r="D40" t="s">
-        <v>407</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>231</v>
+        <v>1031</v>
       </c>
       <c r="B41" t="s">
-        <v>311</v>
+        <v>1110</v>
       </c>
       <c r="C41" t="s">
-        <v>367</v>
+        <v>1165</v>
       </c>
       <c r="D41" t="s">
-        <v>407</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>232</v>
+        <v>1032</v>
       </c>
       <c r="B42" t="s">
-        <v>312</v>
+        <v>1111</v>
       </c>
       <c r="C42" t="s">
-        <v>367</v>
+        <v>1165</v>
       </c>
       <c r="D42" t="s">
-        <v>408</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>233</v>
+        <v>1033</v>
       </c>
       <c r="B43" t="s">
-        <v>313</v>
+        <v>1112</v>
       </c>
       <c r="C43" t="s">
-        <v>368</v>
+        <v>1166</v>
       </c>
       <c r="D43" t="s">
-        <v>409</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>234</v>
+        <v>1034</v>
       </c>
       <c r="B44" t="s">
-        <v>314</v>
+        <v>1113</v>
       </c>
       <c r="C44" t="s">
-        <v>368</v>
+        <v>1166</v>
       </c>
       <c r="D44" t="s">
-        <v>410</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>235</v>
+        <v>1035</v>
       </c>
       <c r="B45" t="s">
-        <v>315</v>
+        <v>1114</v>
       </c>
       <c r="C45" t="s">
-        <v>368</v>
+        <v>1166</v>
       </c>
       <c r="D45" t="s">
-        <v>411</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>236</v>
+        <v>1036</v>
       </c>
       <c r="B46" t="s">
-        <v>316</v>
+        <v>1115</v>
       </c>
       <c r="C46" t="s">
-        <v>368</v>
+        <v>1166</v>
       </c>
       <c r="D46" t="s">
-        <v>412</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>237</v>
+        <v>1037</v>
       </c>
       <c r="B47" t="s">
-        <v>317</v>
+        <v>1116</v>
       </c>
       <c r="C47" t="s">
-        <v>368</v>
+        <v>1166</v>
       </c>
       <c r="D47" t="s">
-        <v>413</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>238</v>
+        <v>1038</v>
       </c>
       <c r="B48" t="s">
-        <v>318</v>
+        <v>1117</v>
       </c>
       <c r="C48" t="s">
-        <v>369</v>
+        <v>1167</v>
       </c>
       <c r="D48" t="s">
-        <v>414</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>239</v>
+        <v>1039</v>
       </c>
       <c r="B49" t="s">
-        <v>319</v>
+        <v>1118</v>
       </c>
       <c r="C49" t="s">
-        <v>369</v>
+        <v>1167</v>
       </c>
       <c r="D49" t="s">
-        <v>415</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>240</v>
+        <v>1040</v>
       </c>
       <c r="B50" t="s">
-        <v>319</v>
+        <v>1118</v>
       </c>
       <c r="C50" t="s">
-        <v>369</v>
+        <v>1167</v>
       </c>
       <c r="D50" t="s">
-        <v>416</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>241</v>
+        <v>1041</v>
       </c>
       <c r="B51" t="s">
-        <v>320</v>
+        <v>1119</v>
       </c>
       <c r="C51" t="s">
-        <v>370</v>
+        <v>1168</v>
       </c>
       <c r="D51" t="s">
-        <v>417</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>242</v>
+        <v>1042</v>
       </c>
       <c r="B52" t="s">
-        <v>321</v>
+        <v>1120</v>
       </c>
       <c r="C52" t="s">
-        <v>371</v>
+        <v>1169</v>
       </c>
       <c r="D52" t="s">
-        <v>418</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>243</v>
+        <v>1043</v>
       </c>
       <c r="B53" t="s">
-        <v>322</v>
+        <v>1121</v>
       </c>
       <c r="C53" t="s">
-        <v>372</v>
+        <v>1169</v>
       </c>
       <c r="D53" t="s">
-        <v>419</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>244</v>
+        <v>1044</v>
       </c>
       <c r="B54" t="s">
-        <v>323</v>
+        <v>1122</v>
       </c>
       <c r="C54" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D54" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>245</v>
+        <v>1045</v>
       </c>
       <c r="B55" t="s">
-        <v>324</v>
+        <v>1123</v>
       </c>
       <c r="C55" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D55" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>246</v>
+        <v>1046</v>
       </c>
       <c r="B56" t="s">
-        <v>325</v>
+        <v>1124</v>
       </c>
       <c r="C56" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D56" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>247</v>
+        <v>1047</v>
       </c>
       <c r="B57" t="s">
-        <v>326</v>
+        <v>1125</v>
       </c>
       <c r="C57" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D57" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>248</v>
+        <v>1048</v>
       </c>
       <c r="B58" t="s">
-        <v>327</v>
+        <v>1126</v>
       </c>
       <c r="C58" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D58" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>249</v>
+        <v>1049</v>
       </c>
       <c r="B59" t="s">
-        <v>328</v>
+        <v>1127</v>
       </c>
       <c r="C59" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D59" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>250</v>
+        <v>1050</v>
       </c>
       <c r="B60" t="s">
-        <v>329</v>
+        <v>1128</v>
       </c>
       <c r="C60" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D60" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>251</v>
+        <v>1051</v>
       </c>
       <c r="B61" t="s">
-        <v>330</v>
+        <v>1129</v>
       </c>
       <c r="C61" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D61" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>252</v>
+        <v>1052</v>
       </c>
       <c r="B62" t="s">
-        <v>331</v>
+        <v>1130</v>
       </c>
       <c r="C62" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D62" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>253</v>
+        <v>1053</v>
       </c>
       <c r="B63" t="s">
-        <v>332</v>
+        <v>1131</v>
       </c>
       <c r="C63" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D63" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>254</v>
+        <v>1054</v>
       </c>
       <c r="B64" t="s">
-        <v>333</v>
+        <v>1132</v>
       </c>
       <c r="C64" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D64" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>255</v>
+        <v>1055</v>
       </c>
       <c r="B65" t="s">
-        <v>334</v>
+        <v>1133</v>
       </c>
       <c r="C65" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D65" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>256</v>
+        <v>1056</v>
       </c>
       <c r="B66" t="s">
-        <v>335</v>
+        <v>1134</v>
       </c>
       <c r="C66" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D66" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>257</v>
+        <v>1057</v>
       </c>
       <c r="B67" t="s">
-        <v>336</v>
+        <v>1135</v>
       </c>
       <c r="C67" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D67" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>258</v>
+        <v>1058</v>
       </c>
       <c r="B68" t="s">
-        <v>337</v>
+        <v>1136</v>
       </c>
       <c r="C68" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D68" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>259</v>
+        <v>1059</v>
       </c>
       <c r="B69" t="s">
-        <v>338</v>
+        <v>1137</v>
       </c>
       <c r="C69" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D69" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>260</v>
+        <v>1060</v>
       </c>
       <c r="B70" t="s">
-        <v>339</v>
+        <v>1138</v>
       </c>
       <c r="C70" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D70" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>261</v>
+        <v>1061</v>
       </c>
       <c r="B71" t="s">
-        <v>340</v>
+        <v>1139</v>
       </c>
       <c r="C71" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D71" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>262</v>
+        <v>1062</v>
       </c>
       <c r="B72" t="s">
-        <v>341</v>
+        <v>1140</v>
       </c>
       <c r="C72" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D72" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>263</v>
+        <v>1063</v>
       </c>
       <c r="B73" t="s">
-        <v>342</v>
+        <v>1141</v>
       </c>
       <c r="C73" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D73" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>264</v>
+        <v>1064</v>
       </c>
       <c r="B74" t="s">
-        <v>343</v>
+        <v>1142</v>
       </c>
       <c r="C74" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D74" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>265</v>
+        <v>1065</v>
       </c>
       <c r="B75" t="s">
-        <v>344</v>
+        <v>1143</v>
       </c>
       <c r="C75" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D75" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>266</v>
+        <v>1066</v>
       </c>
       <c r="B76" t="s">
-        <v>345</v>
+        <v>1144</v>
       </c>
       <c r="C76" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D76" t="s">
-        <v>420</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>267</v>
+        <v>1067</v>
       </c>
       <c r="B77" t="s">
-        <v>346</v>
+        <v>1145</v>
       </c>
       <c r="C77" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D77" t="s">
-        <v>420</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>268</v>
+        <v>1068</v>
       </c>
       <c r="B78" t="s">
-        <v>347</v>
+        <v>1146</v>
       </c>
       <c r="C78" t="s">
-        <v>373</v>
+        <v>1169</v>
       </c>
       <c r="D78" t="s">
-        <v>421</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>269</v>
+        <v>1069</v>
       </c>
       <c r="B79" t="s">
-        <v>348</v>
+        <v>1147</v>
       </c>
       <c r="C79" t="s">
-        <v>373</v>
+        <v>1170</v>
       </c>
       <c r="D79" t="s">
-        <v>422</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>270</v>
+        <v>1070</v>
       </c>
       <c r="B80" t="s">
-        <v>349</v>
+        <v>1148</v>
       </c>
       <c r="C80" t="s">
-        <v>374</v>
+        <v>1171</v>
       </c>
       <c r="D80" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="s">
-        <v>271</v>
-      </c>
-      <c r="B81" t="s">
-        <v>350</v>
-      </c>
-      <c r="C81" t="s">
-        <v>375</v>
-      </c>
-      <c r="D81" t="s">
-        <v>424</v>
+        <v>1219</v>
       </c>
     </row>
   </sheetData>
@@ -2588,167 +4959,167 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>425</v>
+        <v>1220</v>
       </c>
       <c r="B1" t="s">
-        <v>431</v>
+        <v>1226</v>
       </c>
       <c r="C1" t="s">
-        <v>446</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>426</v>
+        <v>1221</v>
       </c>
       <c r="B2" t="s">
-        <v>432</v>
+        <v>1227</v>
       </c>
       <c r="C2" t="s">
-        <v>447</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>426</v>
+        <v>1221</v>
       </c>
       <c r="B3" t="s">
-        <v>433</v>
+        <v>1228</v>
       </c>
       <c r="C3" t="s">
-        <v>448</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>427</v>
+        <v>1222</v>
       </c>
       <c r="B4" t="s">
-        <v>434</v>
+        <v>1229</v>
       </c>
       <c r="C4" t="s">
-        <v>449</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>427</v>
+        <v>1222</v>
       </c>
       <c r="B5" t="s">
-        <v>435</v>
+        <v>1230</v>
       </c>
       <c r="C5" t="s">
-        <v>450</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>428</v>
+        <v>1223</v>
       </c>
       <c r="B6" t="s">
-        <v>436</v>
+        <v>1231</v>
       </c>
       <c r="C6" t="s">
-        <v>451</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>428</v>
+        <v>1223</v>
       </c>
       <c r="B7" t="s">
-        <v>437</v>
+        <v>1232</v>
       </c>
       <c r="C7" t="s">
-        <v>452</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>429</v>
+        <v>1224</v>
       </c>
       <c r="B8" t="s">
-        <v>438</v>
+        <v>1233</v>
       </c>
       <c r="C8" t="s">
-        <v>453</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>429</v>
+        <v>1224</v>
       </c>
       <c r="B9" t="s">
-        <v>439</v>
+        <v>1234</v>
       </c>
       <c r="C9" t="s">
-        <v>454</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>429</v>
+        <v>1224</v>
       </c>
       <c r="B10" t="s">
-        <v>440</v>
+        <v>1235</v>
       </c>
       <c r="C10" t="s">
-        <v>455</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>430</v>
+        <v>1225</v>
       </c>
       <c r="B11" t="s">
-        <v>441</v>
+        <v>1236</v>
       </c>
       <c r="C11" t="s">
-        <v>456</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>430</v>
+        <v>1225</v>
       </c>
       <c r="B12" t="s">
-        <v>442</v>
+        <v>1237</v>
       </c>
       <c r="C12" t="s">
-        <v>457</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>430</v>
+        <v>1225</v>
       </c>
       <c r="B13" t="s">
-        <v>443</v>
+        <v>1238</v>
       </c>
       <c r="C13" t="s">
-        <v>458</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>430</v>
+        <v>1225</v>
       </c>
       <c r="B14" t="s">
-        <v>444</v>
+        <v>1239</v>
       </c>
       <c r="C14" t="s">
-        <v>459</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>430</v>
+        <v>1225</v>
       </c>
       <c r="B15" t="s">
-        <v>445</v>
+        <v>1240</v>
       </c>
       <c r="C15" t="s">
-        <v>460</v>
+        <v>1255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add MDEs to T2 and re-produce
</commit_message>
<xml_diff>
--- a/data/analysis_hh.xlsx
+++ b/data/analysis_hh.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2202" uniqueCount="1256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2936" uniqueCount="1791">
   <si>
     <t>name</t>
   </si>
@@ -3659,6 +3659,1611 @@
   </si>
   <si>
     <t>dead_l</t>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t>perm</t>
+  </si>
+  <si>
+    <t>catyes</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Non-permanent Housing</t>
+  </si>
+  <si>
+    <t>Permanent Housing</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Don't Know</t>
+  </si>
+  <si>
+    <t>Neelum</t>
+  </si>
+  <si>
+    <t>Abbotabad</t>
+  </si>
+  <si>
+    <t>Bagh</t>
+  </si>
+  <si>
+    <t>Mansehra</t>
+  </si>
+  <si>
+    <t>Muzaffarabad</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>censusid</t>
+  </si>
+  <si>
+    <t>hh_assets_pca_post</t>
+  </si>
+  <si>
+    <t>hh_assets_pca_pre</t>
+  </si>
+  <si>
+    <t>hh_consumption_food</t>
+  </si>
+  <si>
+    <t>hh_consumption_nonfood</t>
+  </si>
+  <si>
+    <t>hh_death_eligible</t>
+  </si>
+  <si>
+    <t>hh_district</t>
+  </si>
+  <si>
+    <t>hh_district_1</t>
+  </si>
+  <si>
+    <t>hh_district_2</t>
+  </si>
+  <si>
+    <t>hh_district_3</t>
+  </si>
+  <si>
+    <t>hh_district_4</t>
+  </si>
+  <si>
+    <t>hh_epidist</t>
+  </si>
+  <si>
+    <t>hh_familysize</t>
+  </si>
+  <si>
+    <t>hh_fault_minimum</t>
+  </si>
+  <si>
+    <t>hh_faultdist</t>
+  </si>
+  <si>
+    <t>hh_housing_amount</t>
+  </si>
+  <si>
+    <t>hh_housing_eligible</t>
+  </si>
+  <si>
+    <t>hh_housing_mSec16_q1_trench1</t>
+  </si>
+  <si>
+    <t>hh_injury_eligible</t>
+  </si>
+  <si>
+    <t>hh_lcgs_eligible</t>
+  </si>
+  <si>
+    <t>hh_slope</t>
+  </si>
+  <si>
+    <t>hh_stats_electricity_post</t>
+  </si>
+  <si>
+    <t>hh_stats_electricity_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_govtschool_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_logdistrict_post</t>
+  </si>
+  <si>
+    <t>hh_stats_loggschool_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logmarket_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logmedical_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logprischool_post</t>
+  </si>
+  <si>
+    <t>hh_stats_market_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_medical_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_privateschool_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_water_dist_pre</t>
+  </si>
+  <si>
+    <t>village_code</t>
+  </si>
+  <si>
+    <t>hh_aid_any_1</t>
+  </si>
+  <si>
+    <t>hh_aid_any_2</t>
+  </si>
+  <si>
+    <t>hh_aid_any_3</t>
+  </si>
+  <si>
+    <t>hh_aid_any_4</t>
+  </si>
+  <si>
+    <t>hh_aid_any_5</t>
+  </si>
+  <si>
+    <t>hh_aid_any_6</t>
+  </si>
+  <si>
+    <t>hh_elevation_binary</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_1</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_2</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_4</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_5</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_6</t>
+  </si>
+  <si>
+    <t>hh_far_from_quake</t>
+  </si>
+  <si>
+    <t>hh_perm_house_pre</t>
+  </si>
+  <si>
+    <t>hh_perm_house_post</t>
+  </si>
+  <si>
+    <t>hh_aid_total</t>
+  </si>
+  <si>
+    <t>hh_dead</t>
+  </si>
+  <si>
+    <t>hh_assets_1_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_2_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_3_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_4_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_5_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_6_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_7_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_8_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_9_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_10_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_11_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_12_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_13_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_14_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_15_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_16_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_17_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_18_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_19_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_20_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_21_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_22_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_23_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_24_pre</t>
+  </si>
+  <si>
+    <t>hh_water_inhouse_pre</t>
+  </si>
+  <si>
+    <t>hh_water_inhouse_post</t>
+  </si>
+  <si>
+    <t>hh_infra_index_post</t>
+  </si>
+  <si>
+    <t>tag_uc</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Census ID</t>
+  </si>
+  <si>
+    <t>Asset Index (PCA) (Post-Quake)</t>
+  </si>
+  <si>
+    <t>Asset Index (PCA) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Total Annual Food Expenditure</t>
+  </si>
+  <si>
+    <t>Total Annual Nonfood Expenditure</t>
+  </si>
+  <si>
+    <t>Eligible for death compensation?</t>
+  </si>
+  <si>
+    <t>District Code</t>
+  </si>
+  <si>
+    <t>District Abbottabad</t>
+  </si>
+  <si>
+    <t>District Bagh</t>
+  </si>
+  <si>
+    <t>District Mansehra</t>
+  </si>
+  <si>
+    <t>District Muzaffarabad</t>
+  </si>
+  <si>
+    <t>Distance to Epicenter (km)</t>
+  </si>
+  <si>
+    <t>Family Size</t>
+  </si>
+  <si>
+    <t>Closest Faultline (km)</t>
+  </si>
+  <si>
+    <t>Distance to Faultline (km)</t>
+  </si>
+  <si>
+    <t>Amount received from housing compensation</t>
+  </si>
+  <si>
+    <t>Eligible for housing compensation?</t>
+  </si>
+  <si>
+    <t>Did any member receive 1st trench of 25,000 rupee grant immediately following EQ</t>
+  </si>
+  <si>
+    <t>Eligible for injury compensation?</t>
+  </si>
+  <si>
+    <t>Eligible for lcgs compensation?</t>
+  </si>
+  <si>
+    <t>Mean Slope of UC</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Gov't School (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Log Dist to Distr Office (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Gov't School (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Market (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Medical (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Private School (min)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Market (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Medical Facility (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Private School (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Distance to Water (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Village Code</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Financial</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Health and Medical</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Shelter</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Food</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Supplies</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Liaison with other organizations</t>
+  </si>
+  <si>
+    <t>Above Median Elevation</t>
+  </si>
+  <si>
+    <t>Distance to Water (km)</t>
+  </si>
+  <si>
+    <t>Distance to Health Clinic (km)</t>
+  </si>
+  <si>
+    <t>Distance to Boys School (km)</t>
+  </si>
+  <si>
+    <t>Distance to Girls School (km)</t>
+  </si>
+  <si>
+    <t>Distance to Private School (km)</t>
+  </si>
+  <si>
+    <t>Far from Fault (&gt;20km)</t>
+  </si>
+  <si>
+    <t>Permanent House (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Total Reported Aid Compensation</t>
+  </si>
+  <si>
+    <t>Number Dead in Earthquake</t>
+  </si>
+  <si>
+    <t>Beds/Charpais</t>
+  </si>
+  <si>
+    <t>Tables</t>
+  </si>
+  <si>
+    <t>Chairs</t>
+  </si>
+  <si>
+    <t>Fans (Ceiling/Table/Pedestal/Exhaust)</t>
+  </si>
+  <si>
+    <t>Sewing machine</t>
+  </si>
+  <si>
+    <t>Books</t>
+  </si>
+  <si>
+    <t>Refrigerator</t>
+  </si>
+  <si>
+    <t>Radio/Cassette recorder/CD Player</t>
+  </si>
+  <si>
+    <t>Television</t>
+  </si>
+  <si>
+    <t>VCR/VCD</t>
+  </si>
+  <si>
+    <t>Watches</t>
+  </si>
+  <si>
+    <t>Guns</t>
+  </si>
+  <si>
+    <t>Plough</t>
+  </si>
+  <si>
+    <t>Tractor</t>
+  </si>
+  <si>
+    <t>Tube well/Hand pump</t>
+  </si>
+  <si>
+    <t>Other Agricultural Machinery</t>
+  </si>
+  <si>
+    <t>Other Agricultural Hand-Tools/Saw</t>
+  </si>
+  <si>
+    <t>Motorcycle/Scooter</t>
+  </si>
+  <si>
+    <t>Car/Taxi/Vehicle</t>
+  </si>
+  <si>
+    <t>Bicycle</t>
+  </si>
+  <si>
+    <t>Cattle</t>
+  </si>
+  <si>
+    <t>Goats</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Mobile Phone</t>
+  </si>
+  <si>
+    <t>Water In House (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Water In House (Post-Quake)</t>
+  </si>
+  <si>
+    <t>Household Infrastructure Index</t>
+  </si>
+  <si>
+    <t>Union Council Tag</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>choices</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>catyes</t>
+  </si>
+  <si>
+    <t>hh_elevation_binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>perm</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>dead_l</t>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t>perm</t>
+  </si>
+  <si>
+    <t>catyes</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Non-permanent Housing</t>
+  </si>
+  <si>
+    <t>Permanent Housing</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Don't Know</t>
+  </si>
+  <si>
+    <t>Neelum</t>
+  </si>
+  <si>
+    <t>Abbotabad</t>
+  </si>
+  <si>
+    <t>Bagh</t>
+  </si>
+  <si>
+    <t>Mansehra</t>
+  </si>
+  <si>
+    <t>Muzaffarabad</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>censusid</t>
+  </si>
+  <si>
+    <t>hh_assets_pca_post</t>
+  </si>
+  <si>
+    <t>hh_assets_pca_pre</t>
+  </si>
+  <si>
+    <t>hh_consumption_food</t>
+  </si>
+  <si>
+    <t>hh_consumption_nonfood</t>
+  </si>
+  <si>
+    <t>hh_death_eligible</t>
+  </si>
+  <si>
+    <t>hh_district</t>
+  </si>
+  <si>
+    <t>hh_district_1</t>
+  </si>
+  <si>
+    <t>hh_district_2</t>
+  </si>
+  <si>
+    <t>hh_district_3</t>
+  </si>
+  <si>
+    <t>hh_district_4</t>
+  </si>
+  <si>
+    <t>hh_epidist</t>
+  </si>
+  <si>
+    <t>hh_familysize</t>
+  </si>
+  <si>
+    <t>hh_fault_minimum</t>
+  </si>
+  <si>
+    <t>hh_faultdist</t>
+  </si>
+  <si>
+    <t>hh_housing_amount</t>
+  </si>
+  <si>
+    <t>hh_housing_eligible</t>
+  </si>
+  <si>
+    <t>hh_housing_mSec16_q1_trench1</t>
+  </si>
+  <si>
+    <t>hh_injury_eligible</t>
+  </si>
+  <si>
+    <t>hh_lcgs_eligible</t>
+  </si>
+  <si>
+    <t>hh_slope</t>
+  </si>
+  <si>
+    <t>hh_stats_electricity_post</t>
+  </si>
+  <si>
+    <t>hh_stats_electricity_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_govtschool_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_logdistrict_post</t>
+  </si>
+  <si>
+    <t>hh_stats_loggschool_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logmarket_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logmedical_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logprischool_post</t>
+  </si>
+  <si>
+    <t>hh_stats_market_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_medical_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_privateschool_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_water_dist_pre</t>
+  </si>
+  <si>
+    <t>village_code</t>
+  </si>
+  <si>
+    <t>hh_aid_any_1</t>
+  </si>
+  <si>
+    <t>hh_aid_any_2</t>
+  </si>
+  <si>
+    <t>hh_aid_any_3</t>
+  </si>
+  <si>
+    <t>hh_aid_any_4</t>
+  </si>
+  <si>
+    <t>hh_aid_any_5</t>
+  </si>
+  <si>
+    <t>hh_aid_any_6</t>
+  </si>
+  <si>
+    <t>hh_elevation_binary</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_1</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_2</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_4</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_5</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_6</t>
+  </si>
+  <si>
+    <t>hh_far_from_quake</t>
+  </si>
+  <si>
+    <t>hh_perm_house_pre</t>
+  </si>
+  <si>
+    <t>hh_perm_house_post</t>
+  </si>
+  <si>
+    <t>hh_aid_total</t>
+  </si>
+  <si>
+    <t>hh_dead</t>
+  </si>
+  <si>
+    <t>hh_logconscap</t>
+  </si>
+  <si>
+    <t>hh_assets_1_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_2_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_3_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_4_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_5_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_6_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_7_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_8_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_9_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_10_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_11_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_12_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_13_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_14_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_15_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_16_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_17_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_18_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_19_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_20_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_21_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_22_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_23_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_24_pre</t>
+  </si>
+  <si>
+    <t>hh_water_inhouse_pre</t>
+  </si>
+  <si>
+    <t>hh_water_inhouse_post</t>
+  </si>
+  <si>
+    <t>hh_infra_index_post</t>
+  </si>
+  <si>
+    <t>tag_uc</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Census ID</t>
+  </si>
+  <si>
+    <t>Asset Index (PCA) (Post-Quake)</t>
+  </si>
+  <si>
+    <t>Asset Index (PCA) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Total Annual Food Expenditure</t>
+  </si>
+  <si>
+    <t>Total Annual Nonfood Expenditure</t>
+  </si>
+  <si>
+    <t>Eligible for death compensation?</t>
+  </si>
+  <si>
+    <t>District Code</t>
+  </si>
+  <si>
+    <t>District Abbottabad</t>
+  </si>
+  <si>
+    <t>District Bagh</t>
+  </si>
+  <si>
+    <t>District Mansehra</t>
+  </si>
+  <si>
+    <t>District Muzaffarabad</t>
+  </si>
+  <si>
+    <t>Distance to Epicenter (km)</t>
+  </si>
+  <si>
+    <t>Family Size</t>
+  </si>
+  <si>
+    <t>Closest Faultline (km)</t>
+  </si>
+  <si>
+    <t>Distance to Faultline (km)</t>
+  </si>
+  <si>
+    <t>Amount received from housing compensation</t>
+  </si>
+  <si>
+    <t>Eligible for housing compensation?</t>
+  </si>
+  <si>
+    <t>Did any member receive 1st trench of 25,000 rupee grant immediately following EQ</t>
+  </si>
+  <si>
+    <t>Eligible for injury compensation?</t>
+  </si>
+  <si>
+    <t>Eligible for lcgs compensation?</t>
+  </si>
+  <si>
+    <t>Mean Slope of UC</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Gov't School (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Log Dist to Distr Office (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Gov't School (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Market (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Medical (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Private School (min)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Market (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Medical Facility (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Private School (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Distance to Water (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Village Code</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Financial</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Health and Medical</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Shelter</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Food</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Supplies</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Liaison with other organizations</t>
+  </si>
+  <si>
+    <t>Above Median Elevation</t>
+  </si>
+  <si>
+    <t>Distance to Water (km)</t>
+  </si>
+  <si>
+    <t>Distance to Health Clinic (km)</t>
+  </si>
+  <si>
+    <t>Distance to Boys School (km)</t>
+  </si>
+  <si>
+    <t>Distance to Girls School (km)</t>
+  </si>
+  <si>
+    <t>Distance to Private School (km)</t>
+  </si>
+  <si>
+    <t>Far from Fault (&gt;20km)</t>
+  </si>
+  <si>
+    <t>Permanent House (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Total Reported Aid Compensation</t>
+  </si>
+  <si>
+    <t>Number Dead in Earthquake</t>
+  </si>
+  <si>
+    <t>(log) Consumption per Capita</t>
+  </si>
+  <si>
+    <t>Beds/Charpais</t>
+  </si>
+  <si>
+    <t>Tables</t>
+  </si>
+  <si>
+    <t>Chairs</t>
+  </si>
+  <si>
+    <t>Fans (Ceiling/Table/Pedestal/Exhaust)</t>
+  </si>
+  <si>
+    <t>Sewing machine</t>
+  </si>
+  <si>
+    <t>Books</t>
+  </si>
+  <si>
+    <t>Refrigerator</t>
+  </si>
+  <si>
+    <t>Radio/Cassette recorder/CD Player</t>
+  </si>
+  <si>
+    <t>Television</t>
+  </si>
+  <si>
+    <t>VCR/VCD</t>
+  </si>
+  <si>
+    <t>Watches</t>
+  </si>
+  <si>
+    <t>Guns</t>
+  </si>
+  <si>
+    <t>Plough</t>
+  </si>
+  <si>
+    <t>Tractor</t>
+  </si>
+  <si>
+    <t>Tube well/Hand pump</t>
+  </si>
+  <si>
+    <t>Other Agricultural Machinery</t>
+  </si>
+  <si>
+    <t>Other Agricultural Hand-Tools/Saw</t>
+  </si>
+  <si>
+    <t>Motorcycle/Scooter</t>
+  </si>
+  <si>
+    <t>Car/Taxi/Vehicle</t>
+  </si>
+  <si>
+    <t>Bicycle</t>
+  </si>
+  <si>
+    <t>Cattle</t>
+  </si>
+  <si>
+    <t>Goats</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Mobile Phone</t>
+  </si>
+  <si>
+    <t>Water In House (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Water In House (Post-Quake)</t>
+  </si>
+  <si>
+    <t>Household Infrastructure Index</t>
+  </si>
+  <si>
+    <t>Union Council Tag</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>choices</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>catyes</t>
+  </si>
+  <si>
+    <t>hh_elevation_binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>perm</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>dead_l</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>yesno</t>
@@ -3825,1127 +5430,1141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D81"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>991</v>
+        <v>1521</v>
       </c>
       <c r="B1" t="s">
-        <v>1071</v>
+        <v>1602</v>
       </c>
       <c r="C1" t="s">
-        <v>1149</v>
+        <v>1681</v>
       </c>
       <c r="D1" t="s">
-        <v>1172</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>992</v>
+        <v>1522</v>
       </c>
       <c r="B2" t="s">
-        <v>1072</v>
+        <v>1603</v>
       </c>
       <c r="C2" t="s">
-        <v>1150</v>
+        <v>1682</v>
       </c>
       <c r="D2" t="s">
-        <v>1173</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>993</v>
+        <v>1523</v>
       </c>
       <c r="B3" t="s">
-        <v>1073</v>
+        <v>1604</v>
       </c>
       <c r="C3" t="s">
-        <v>1151</v>
+        <v>1683</v>
       </c>
       <c r="D3" t="s">
-        <v>1174</v>
+        <v>1708</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>994</v>
+        <v>1524</v>
       </c>
       <c r="B4" t="s">
-        <v>1074</v>
+        <v>1605</v>
       </c>
       <c r="C4" t="s">
-        <v>1151</v>
+        <v>1683</v>
       </c>
       <c r="D4" t="s">
-        <v>1175</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>995</v>
+        <v>1525</v>
       </c>
       <c r="B5" t="s">
-        <v>1075</v>
+        <v>1606</v>
       </c>
       <c r="C5" t="s">
-        <v>1151</v>
+        <v>1683</v>
       </c>
       <c r="D5" t="s">
-        <v>1176</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>996</v>
+        <v>1526</v>
       </c>
       <c r="B6" t="s">
-        <v>1076</v>
+        <v>1607</v>
       </c>
       <c r="C6" t="s">
-        <v>1151</v>
+        <v>1683</v>
       </c>
       <c r="D6" t="s">
-        <v>1177</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>997</v>
+        <v>1527</v>
       </c>
       <c r="B7" t="s">
-        <v>1077</v>
+        <v>1608</v>
       </c>
       <c r="C7" t="s">
-        <v>1152</v>
+        <v>1684</v>
       </c>
       <c r="D7" t="s">
-        <v>1178</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>998</v>
+        <v>1528</v>
       </c>
       <c r="B8" t="s">
-        <v>1078</v>
+        <v>1609</v>
       </c>
       <c r="C8" t="s">
-        <v>1152</v>
+        <v>1684</v>
       </c>
       <c r="D8" t="s">
-        <v>1179</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>999</v>
+        <v>1529</v>
       </c>
       <c r="B9" t="s">
-        <v>1079</v>
+        <v>1610</v>
       </c>
       <c r="C9" t="s">
-        <v>1152</v>
+        <v>1684</v>
       </c>
       <c r="D9" t="s">
-        <v>1180</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>1000</v>
+        <v>1530</v>
       </c>
       <c r="B10" t="s">
-        <v>1080</v>
+        <v>1611</v>
       </c>
       <c r="C10" t="s">
-        <v>1152</v>
+        <v>1684</v>
       </c>
       <c r="D10" t="s">
-        <v>1181</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>1001</v>
+        <v>1531</v>
       </c>
       <c r="B11" t="s">
-        <v>1081</v>
+        <v>1612</v>
       </c>
       <c r="C11" t="s">
-        <v>1152</v>
+        <v>1684</v>
       </c>
       <c r="D11" t="s">
-        <v>1182</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>1002</v>
+        <v>1532</v>
       </c>
       <c r="B12" t="s">
-        <v>1082</v>
+        <v>1613</v>
       </c>
       <c r="C12" t="s">
-        <v>1152</v>
+        <v>1684</v>
       </c>
       <c r="D12" t="s">
-        <v>1183</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>1003</v>
+        <v>1533</v>
       </c>
       <c r="B13" t="s">
-        <v>1083</v>
+        <v>1614</v>
       </c>
       <c r="C13" t="s">
-        <v>1153</v>
+        <v>1685</v>
       </c>
       <c r="D13" t="s">
-        <v>1184</v>
+        <v>1718</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>1004</v>
+        <v>1534</v>
       </c>
       <c r="B14" t="s">
-        <v>1084</v>
+        <v>1615</v>
       </c>
       <c r="C14" t="s">
-        <v>1154</v>
+        <v>1686</v>
       </c>
       <c r="D14" t="s">
-        <v>1185</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>1005</v>
+        <v>1535</v>
       </c>
       <c r="B15" t="s">
-        <v>1085</v>
+        <v>1616</v>
       </c>
       <c r="C15" t="s">
-        <v>1155</v>
+        <v>1687</v>
       </c>
       <c r="D15" t="s">
-        <v>1186</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>1006</v>
+        <v>1536</v>
       </c>
       <c r="B16" t="s">
-        <v>1086</v>
+        <v>1617</v>
       </c>
       <c r="C16" t="s">
-        <v>1155</v>
+        <v>1687</v>
       </c>
       <c r="D16" t="s">
-        <v>1187</v>
+        <v>1721</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>1007</v>
+        <v>1537</v>
       </c>
       <c r="B17" t="s">
-        <v>1087</v>
+        <v>1618</v>
       </c>
       <c r="C17" t="s">
-        <v>1156</v>
+        <v>1688</v>
       </c>
       <c r="D17" t="s">
-        <v>1188</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>1008</v>
+        <v>1538</v>
       </c>
       <c r="B18" t="s">
-        <v>1088</v>
+        <v>1619</v>
       </c>
       <c r="C18" t="s">
-        <v>1157</v>
+        <v>1689</v>
       </c>
       <c r="D18" t="s">
-        <v>1189</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>1009</v>
+        <v>1539</v>
       </c>
       <c r="B19" t="s">
-        <v>1089</v>
+        <v>1620</v>
       </c>
       <c r="C19" t="s">
-        <v>1157</v>
+        <v>1689</v>
       </c>
       <c r="D19" t="s">
-        <v>1189</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>1010</v>
+        <v>1540</v>
       </c>
       <c r="B20" t="s">
-        <v>1090</v>
+        <v>1621</v>
       </c>
       <c r="C20" t="s">
-        <v>1157</v>
+        <v>1689</v>
       </c>
       <c r="D20" t="s">
-        <v>1189</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>1011</v>
+        <v>1541</v>
       </c>
       <c r="B21" t="s">
-        <v>1091</v>
+        <v>1622</v>
       </c>
       <c r="C21" t="s">
-        <v>1157</v>
+        <v>1689</v>
       </c>
       <c r="D21" t="s">
-        <v>1189</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>1012</v>
+        <v>1542</v>
       </c>
       <c r="B22" t="s">
-        <v>1092</v>
+        <v>1623</v>
       </c>
       <c r="C22" t="s">
-        <v>1158</v>
+        <v>1690</v>
       </c>
       <c r="D22" t="s">
-        <v>1190</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>1013</v>
+        <v>1543</v>
       </c>
       <c r="B23" t="s">
-        <v>1093</v>
+        <v>1624</v>
       </c>
       <c r="C23" t="s">
-        <v>1159</v>
+        <v>1691</v>
       </c>
       <c r="D23" t="s">
-        <v>1191</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>1014</v>
+        <v>1544</v>
       </c>
       <c r="B24" t="s">
-        <v>1093</v>
+        <v>1624</v>
       </c>
       <c r="C24" t="s">
-        <v>1159</v>
+        <v>1691</v>
       </c>
       <c r="D24" t="s">
-        <v>1191</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>1015</v>
+        <v>1545</v>
       </c>
       <c r="B25" t="s">
-        <v>1094</v>
+        <v>1625</v>
       </c>
       <c r="C25" t="s">
-        <v>1160</v>
+        <v>1692</v>
       </c>
       <c r="D25" t="s">
-        <v>1192</v>
+        <v>1726</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>1016</v>
+        <v>1546</v>
       </c>
       <c r="B26" t="s">
-        <v>1095</v>
+        <v>1626</v>
       </c>
       <c r="C26" t="s">
-        <v>1161</v>
+        <v>1693</v>
       </c>
       <c r="D26" t="s">
-        <v>1193</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>1017</v>
+        <v>1547</v>
       </c>
       <c r="B27" t="s">
-        <v>1096</v>
+        <v>1627</v>
       </c>
       <c r="C27" t="s">
-        <v>1161</v>
+        <v>1693</v>
       </c>
       <c r="D27" t="s">
-        <v>1194</v>
+        <v>1728</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>1018</v>
+        <v>1548</v>
       </c>
       <c r="B28" t="s">
-        <v>1097</v>
+        <v>1628</v>
       </c>
       <c r="C28" t="s">
-        <v>1161</v>
+        <v>1693</v>
       </c>
       <c r="D28" t="s">
-        <v>1195</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>1019</v>
+        <v>1549</v>
       </c>
       <c r="B29" t="s">
-        <v>1098</v>
+        <v>1629</v>
       </c>
       <c r="C29" t="s">
-        <v>1161</v>
+        <v>1693</v>
       </c>
       <c r="D29" t="s">
-        <v>1196</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>1020</v>
+        <v>1550</v>
       </c>
       <c r="B30" t="s">
-        <v>1099</v>
+        <v>1630</v>
       </c>
       <c r="C30" t="s">
-        <v>1161</v>
+        <v>1693</v>
       </c>
       <c r="D30" t="s">
-        <v>1197</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>1021</v>
+        <v>1551</v>
       </c>
       <c r="B31" t="s">
-        <v>1100</v>
+        <v>1631</v>
       </c>
       <c r="C31" t="s">
-        <v>1162</v>
+        <v>1694</v>
       </c>
       <c r="D31" t="s">
-        <v>1198</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>1022</v>
+        <v>1552</v>
       </c>
       <c r="B32" t="s">
-        <v>1101</v>
+        <v>1632</v>
       </c>
       <c r="C32" t="s">
-        <v>1162</v>
+        <v>1694</v>
       </c>
       <c r="D32" t="s">
-        <v>1199</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>1023</v>
+        <v>1553</v>
       </c>
       <c r="B33" t="s">
-        <v>1102</v>
+        <v>1633</v>
       </c>
       <c r="C33" t="s">
-        <v>1162</v>
+        <v>1694</v>
       </c>
       <c r="D33" t="s">
-        <v>1200</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>1024</v>
+        <v>1554</v>
       </c>
       <c r="B34" t="s">
-        <v>1103</v>
+        <v>1634</v>
       </c>
       <c r="C34" t="s">
-        <v>1163</v>
+        <v>1695</v>
       </c>
       <c r="D34" t="s">
-        <v>1201</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>1025</v>
+        <v>1555</v>
       </c>
       <c r="B35" t="s">
-        <v>1104</v>
+        <v>1635</v>
       </c>
       <c r="C35" t="s">
-        <v>1164</v>
+        <v>1696</v>
       </c>
       <c r="D35" t="s">
-        <v>1202</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>1026</v>
+        <v>1556</v>
       </c>
       <c r="B36" t="s">
-        <v>1105</v>
+        <v>1636</v>
       </c>
       <c r="C36" t="s">
-        <v>1165</v>
+        <v>1697</v>
       </c>
       <c r="D36" t="s">
-        <v>1203</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>1027</v>
+        <v>1557</v>
       </c>
       <c r="B37" t="s">
-        <v>1106</v>
+        <v>1637</v>
       </c>
       <c r="C37" t="s">
-        <v>1165</v>
+        <v>1697</v>
       </c>
       <c r="D37" t="s">
-        <v>1203</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>1028</v>
+        <v>1558</v>
       </c>
       <c r="B38" t="s">
-        <v>1107</v>
+        <v>1638</v>
       </c>
       <c r="C38" t="s">
-        <v>1165</v>
+        <v>1697</v>
       </c>
       <c r="D38" t="s">
-        <v>1203</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>1029</v>
+        <v>1559</v>
       </c>
       <c r="B39" t="s">
-        <v>1108</v>
+        <v>1639</v>
       </c>
       <c r="C39" t="s">
-        <v>1165</v>
+        <v>1697</v>
       </c>
       <c r="D39" t="s">
-        <v>1203</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>1030</v>
+        <v>1560</v>
       </c>
       <c r="B40" t="s">
-        <v>1109</v>
+        <v>1640</v>
       </c>
       <c r="C40" t="s">
-        <v>1165</v>
+        <v>1697</v>
       </c>
       <c r="D40" t="s">
-        <v>1203</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>1031</v>
+        <v>1561</v>
       </c>
       <c r="B41" t="s">
-        <v>1110</v>
+        <v>1641</v>
       </c>
       <c r="C41" t="s">
-        <v>1165</v>
+        <v>1697</v>
       </c>
       <c r="D41" t="s">
-        <v>1203</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>1032</v>
+        <v>1562</v>
       </c>
       <c r="B42" t="s">
-        <v>1111</v>
+        <v>1642</v>
       </c>
       <c r="C42" t="s">
-        <v>1165</v>
+        <v>1697</v>
       </c>
       <c r="D42" t="s">
-        <v>1204</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>1033</v>
+        <v>1563</v>
       </c>
       <c r="B43" t="s">
-        <v>1112</v>
+        <v>1643</v>
       </c>
       <c r="C43" t="s">
-        <v>1166</v>
+        <v>1698</v>
       </c>
       <c r="D43" t="s">
-        <v>1205</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>1034</v>
+        <v>1564</v>
       </c>
       <c r="B44" t="s">
-        <v>1113</v>
+        <v>1644</v>
       </c>
       <c r="C44" t="s">
-        <v>1166</v>
+        <v>1698</v>
       </c>
       <c r="D44" t="s">
-        <v>1206</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>1035</v>
+        <v>1565</v>
       </c>
       <c r="B45" t="s">
-        <v>1114</v>
+        <v>1645</v>
       </c>
       <c r="C45" t="s">
-        <v>1166</v>
+        <v>1698</v>
       </c>
       <c r="D45" t="s">
-        <v>1207</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>1036</v>
+        <v>1566</v>
       </c>
       <c r="B46" t="s">
-        <v>1115</v>
+        <v>1646</v>
       </c>
       <c r="C46" t="s">
-        <v>1166</v>
+        <v>1698</v>
       </c>
       <c r="D46" t="s">
-        <v>1208</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>1037</v>
+        <v>1567</v>
       </c>
       <c r="B47" t="s">
-        <v>1116</v>
+        <v>1647</v>
       </c>
       <c r="C47" t="s">
-        <v>1166</v>
+        <v>1698</v>
       </c>
       <c r="D47" t="s">
-        <v>1209</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>1038</v>
+        <v>1568</v>
       </c>
       <c r="B48" t="s">
-        <v>1117</v>
+        <v>1648</v>
       </c>
       <c r="C48" t="s">
-        <v>1167</v>
+        <v>1699</v>
       </c>
       <c r="D48" t="s">
-        <v>1210</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>1039</v>
+        <v>1569</v>
       </c>
       <c r="B49" t="s">
-        <v>1118</v>
+        <v>1649</v>
       </c>
       <c r="C49" t="s">
-        <v>1167</v>
+        <v>1699</v>
       </c>
       <c r="D49" t="s">
-        <v>1211</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>1040</v>
+        <v>1570</v>
       </c>
       <c r="B50" t="s">
-        <v>1118</v>
+        <v>1649</v>
       </c>
       <c r="C50" t="s">
-        <v>1167</v>
+        <v>1699</v>
       </c>
       <c r="D50" t="s">
-        <v>1212</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>1041</v>
+        <v>1571</v>
       </c>
       <c r="B51" t="s">
-        <v>1119</v>
+        <v>1650</v>
       </c>
       <c r="C51" t="s">
-        <v>1168</v>
+        <v>1700</v>
       </c>
       <c r="D51" t="s">
-        <v>1213</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>1042</v>
+        <v>1572</v>
       </c>
       <c r="B52" t="s">
-        <v>1120</v>
+        <v>1651</v>
       </c>
       <c r="C52" t="s">
-        <v>1169</v>
+        <v>1701</v>
       </c>
       <c r="D52" t="s">
-        <v>1214</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>1043</v>
+        <v>1573</v>
       </c>
       <c r="B53" t="s">
-        <v>1121</v>
+        <v>1652</v>
       </c>
       <c r="C53" t="s">
-        <v>1169</v>
+        <v>1702</v>
       </c>
       <c r="D53" t="s">
-        <v>1215</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>1044</v>
+        <v>1574</v>
       </c>
       <c r="B54" t="s">
-        <v>1122</v>
+        <v>1653</v>
       </c>
       <c r="C54" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D54" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>1045</v>
+        <v>1575</v>
       </c>
       <c r="B55" t="s">
-        <v>1123</v>
+        <v>1654</v>
       </c>
       <c r="C55" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D55" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>1046</v>
+        <v>1576</v>
       </c>
       <c r="B56" t="s">
-        <v>1124</v>
+        <v>1655</v>
       </c>
       <c r="C56" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D56" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>1047</v>
+        <v>1577</v>
       </c>
       <c r="B57" t="s">
-        <v>1125</v>
+        <v>1656</v>
       </c>
       <c r="C57" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D57" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>1048</v>
+        <v>1578</v>
       </c>
       <c r="B58" t="s">
-        <v>1126</v>
+        <v>1657</v>
       </c>
       <c r="C58" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D58" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>1049</v>
+        <v>1579</v>
       </c>
       <c r="B59" t="s">
-        <v>1127</v>
+        <v>1658</v>
       </c>
       <c r="C59" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D59" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>1050</v>
+        <v>1580</v>
       </c>
       <c r="B60" t="s">
-        <v>1128</v>
+        <v>1659</v>
       </c>
       <c r="C60" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D60" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>1051</v>
+        <v>1581</v>
       </c>
       <c r="B61" t="s">
-        <v>1129</v>
+        <v>1660</v>
       </c>
       <c r="C61" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D61" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>1052</v>
+        <v>1582</v>
       </c>
       <c r="B62" t="s">
-        <v>1130</v>
+        <v>1661</v>
       </c>
       <c r="C62" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D62" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>1053</v>
+        <v>1583</v>
       </c>
       <c r="B63" t="s">
-        <v>1131</v>
+        <v>1662</v>
       </c>
       <c r="C63" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D63" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>1054</v>
+        <v>1584</v>
       </c>
       <c r="B64" t="s">
-        <v>1132</v>
+        <v>1663</v>
       </c>
       <c r="C64" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D64" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>1055</v>
+        <v>1585</v>
       </c>
       <c r="B65" t="s">
-        <v>1133</v>
+        <v>1664</v>
       </c>
       <c r="C65" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D65" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>1056</v>
+        <v>1586</v>
       </c>
       <c r="B66" t="s">
-        <v>1134</v>
+        <v>1665</v>
       </c>
       <c r="C66" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D66" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>1057</v>
+        <v>1587</v>
       </c>
       <c r="B67" t="s">
-        <v>1135</v>
+        <v>1666</v>
       </c>
       <c r="C67" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D67" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>1058</v>
+        <v>1588</v>
       </c>
       <c r="B68" t="s">
-        <v>1136</v>
+        <v>1667</v>
       </c>
       <c r="C68" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D68" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>1059</v>
+        <v>1589</v>
       </c>
       <c r="B69" t="s">
-        <v>1137</v>
+        <v>1668</v>
       </c>
       <c r="C69" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D69" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>1060</v>
+        <v>1590</v>
       </c>
       <c r="B70" t="s">
-        <v>1138</v>
+        <v>1669</v>
       </c>
       <c r="C70" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D70" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>1061</v>
+        <v>1591</v>
       </c>
       <c r="B71" t="s">
-        <v>1139</v>
+        <v>1670</v>
       </c>
       <c r="C71" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D71" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>1062</v>
+        <v>1592</v>
       </c>
       <c r="B72" t="s">
-        <v>1140</v>
+        <v>1671</v>
       </c>
       <c r="C72" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D72" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>1063</v>
+        <v>1593</v>
       </c>
       <c r="B73" t="s">
-        <v>1141</v>
+        <v>1672</v>
       </c>
       <c r="C73" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D73" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>1064</v>
+        <v>1594</v>
       </c>
       <c r="B74" t="s">
-        <v>1142</v>
+        <v>1673</v>
       </c>
       <c r="C74" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D74" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>1065</v>
+        <v>1595</v>
       </c>
       <c r="B75" t="s">
-        <v>1143</v>
+        <v>1674</v>
       </c>
       <c r="C75" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D75" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>1066</v>
+        <v>1596</v>
       </c>
       <c r="B76" t="s">
-        <v>1144</v>
+        <v>1675</v>
       </c>
       <c r="C76" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D76" t="s">
-        <v>1215</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>1067</v>
+        <v>1597</v>
       </c>
       <c r="B77" t="s">
-        <v>1145</v>
+        <v>1676</v>
       </c>
       <c r="C77" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D77" t="s">
-        <v>1216</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>1068</v>
+        <v>1598</v>
       </c>
       <c r="B78" t="s">
-        <v>1146</v>
+        <v>1677</v>
       </c>
       <c r="C78" t="s">
-        <v>1169</v>
+        <v>1703</v>
       </c>
       <c r="D78" t="s">
-        <v>1217</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>1069</v>
+        <v>1599</v>
       </c>
       <c r="B79" t="s">
-        <v>1147</v>
+        <v>1678</v>
       </c>
       <c r="C79" t="s">
-        <v>1170</v>
+        <v>1703</v>
       </c>
       <c r="D79" t="s">
-        <v>1218</v>
+        <v>1752</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>1070</v>
+        <v>1600</v>
       </c>
       <c r="B80" t="s">
-        <v>1148</v>
+        <v>1679</v>
       </c>
       <c r="C80" t="s">
-        <v>1171</v>
+        <v>1704</v>
       </c>
       <c r="D80" t="s">
-        <v>1219</v>
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>1601</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1680</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1705</v>
+      </c>
+      <c r="D81" t="s">
+        <v>1754</v>
       </c>
     </row>
   </sheetData>
@@ -4959,167 +6578,167 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>1220</v>
+        <v>1755</v>
       </c>
       <c r="B1" t="s">
-        <v>1226</v>
+        <v>1761</v>
       </c>
       <c r="C1" t="s">
-        <v>1241</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1221</v>
+        <v>1756</v>
       </c>
       <c r="B2" t="s">
-        <v>1227</v>
+        <v>1762</v>
       </c>
       <c r="C2" t="s">
-        <v>1242</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>1221</v>
+        <v>1756</v>
       </c>
       <c r="B3" t="s">
-        <v>1228</v>
+        <v>1763</v>
       </c>
       <c r="C3" t="s">
-        <v>1243</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>1222</v>
+        <v>1757</v>
       </c>
       <c r="B4" t="s">
-        <v>1229</v>
+        <v>1764</v>
       </c>
       <c r="C4" t="s">
-        <v>1244</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>1222</v>
+        <v>1757</v>
       </c>
       <c r="B5" t="s">
-        <v>1230</v>
+        <v>1765</v>
       </c>
       <c r="C5" t="s">
-        <v>1245</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>1223</v>
+        <v>1758</v>
       </c>
       <c r="B6" t="s">
-        <v>1231</v>
+        <v>1766</v>
       </c>
       <c r="C6" t="s">
-        <v>1246</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>1223</v>
+        <v>1758</v>
       </c>
       <c r="B7" t="s">
-        <v>1232</v>
+        <v>1767</v>
       </c>
       <c r="C7" t="s">
-        <v>1247</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>1224</v>
+        <v>1759</v>
       </c>
       <c r="B8" t="s">
-        <v>1233</v>
+        <v>1768</v>
       </c>
       <c r="C8" t="s">
-        <v>1248</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>1224</v>
+        <v>1759</v>
       </c>
       <c r="B9" t="s">
-        <v>1234</v>
+        <v>1769</v>
       </c>
       <c r="C9" t="s">
-        <v>1249</v>
+        <v>1784</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>1224</v>
+        <v>1759</v>
       </c>
       <c r="B10" t="s">
-        <v>1235</v>
+        <v>1770</v>
       </c>
       <c r="C10" t="s">
-        <v>1250</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>1225</v>
+        <v>1760</v>
       </c>
       <c r="B11" t="s">
-        <v>1236</v>
+        <v>1771</v>
       </c>
       <c r="C11" t="s">
-        <v>1251</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>1225</v>
+        <v>1760</v>
       </c>
       <c r="B12" t="s">
-        <v>1237</v>
+        <v>1772</v>
       </c>
       <c r="C12" t="s">
-        <v>1252</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>1225</v>
+        <v>1760</v>
       </c>
       <c r="B13" t="s">
-        <v>1238</v>
+        <v>1773</v>
       </c>
       <c r="C13" t="s">
-        <v>1253</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>1225</v>
+        <v>1760</v>
       </c>
       <c r="B14" t="s">
-        <v>1239</v>
+        <v>1774</v>
       </c>
       <c r="C14" t="s">
-        <v>1254</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>1225</v>
+        <v>1760</v>
       </c>
       <c r="B15" t="s">
-        <v>1240</v>
+        <v>1775</v>
       </c>
       <c r="C15" t="s">
-        <v>1255</v>
+        <v>1790</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add school density and occupation data
</commit_message>
<xml_diff>
--- a/data/analysis_hh.xlsx
+++ b/data/analysis_hh.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3305" uniqueCount="2061">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4043" uniqueCount="2601">
   <si>
     <t>name</t>
   </si>
@@ -4454,6 +4454,1626 @@
   </si>
   <si>
     <t>dead_l</t>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t>perm</t>
+  </si>
+  <si>
+    <t>catyes</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Non-permanent Housing</t>
+  </si>
+  <si>
+    <t>Permanent Housing</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Don't Know</t>
+  </si>
+  <si>
+    <t>Neelum</t>
+  </si>
+  <si>
+    <t>Abbotabad</t>
+  </si>
+  <si>
+    <t>Bagh</t>
+  </si>
+  <si>
+    <t>Mansehra</t>
+  </si>
+  <si>
+    <t>Muzaffarabad</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>censusid</t>
+  </si>
+  <si>
+    <t>hh_assets_pca_post</t>
+  </si>
+  <si>
+    <t>hh_assets_pca_pre</t>
+  </si>
+  <si>
+    <t>hh_consumption_food</t>
+  </si>
+  <si>
+    <t>hh_consumption_nonfood</t>
+  </si>
+  <si>
+    <t>hh_death_eligible</t>
+  </si>
+  <si>
+    <t>hh_district</t>
+  </si>
+  <si>
+    <t>hh_district_1</t>
+  </si>
+  <si>
+    <t>hh_district_2</t>
+  </si>
+  <si>
+    <t>hh_district_3</t>
+  </si>
+  <si>
+    <t>hh_district_4</t>
+  </si>
+  <si>
+    <t>hh_epidist</t>
+  </si>
+  <si>
+    <t>hh_familysize</t>
+  </si>
+  <si>
+    <t>hh_fault_minimum</t>
+  </si>
+  <si>
+    <t>hh_faultdist</t>
+  </si>
+  <si>
+    <t>hh_housing_amount</t>
+  </si>
+  <si>
+    <t>hh_housing_eligible</t>
+  </si>
+  <si>
+    <t>hh_housing_mSec16_q1_trench1</t>
+  </si>
+  <si>
+    <t>hh_injury_eligible</t>
+  </si>
+  <si>
+    <t>hh_lcgs_eligible</t>
+  </si>
+  <si>
+    <t>hh_slope</t>
+  </si>
+  <si>
+    <t>hh_stats_electricity_post</t>
+  </si>
+  <si>
+    <t>hh_stats_electricity_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_govtschool_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_logdistrict_post</t>
+  </si>
+  <si>
+    <t>hh_stats_loggschool_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logmarket_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logmedical_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logprischool_post</t>
+  </si>
+  <si>
+    <t>hh_stats_market_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_medical_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_privateschool_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_water_dist_pre</t>
+  </si>
+  <si>
+    <t>village_code</t>
+  </si>
+  <si>
+    <t>hh_aid_any_1</t>
+  </si>
+  <si>
+    <t>hh_aid_any_2</t>
+  </si>
+  <si>
+    <t>hh_aid_any_3</t>
+  </si>
+  <si>
+    <t>hh_aid_any_4</t>
+  </si>
+  <si>
+    <t>hh_aid_any_5</t>
+  </si>
+  <si>
+    <t>hh_aid_any_6</t>
+  </si>
+  <si>
+    <t>hh_elevation_binary</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_1</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_2</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_4</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_5</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_6</t>
+  </si>
+  <si>
+    <t>hh_far_from_quake</t>
+  </si>
+  <si>
+    <t>hh_perm_house_pre</t>
+  </si>
+  <si>
+    <t>hh_perm_house_post</t>
+  </si>
+  <si>
+    <t>hh_aid_total</t>
+  </si>
+  <si>
+    <t>hh_dead</t>
+  </si>
+  <si>
+    <t>hh_logconscap</t>
+  </si>
+  <si>
+    <t>hh_assets_1_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_2_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_3_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_4_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_5_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_6_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_7_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_8_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_9_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_10_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_11_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_12_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_13_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_14_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_15_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_16_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_17_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_18_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_19_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_20_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_21_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_22_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_23_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_24_pre</t>
+  </si>
+  <si>
+    <t>hh_water_inhouse_pre</t>
+  </si>
+  <si>
+    <t>hh_water_inhouse_post</t>
+  </si>
+  <si>
+    <t>hh_infra_index_post</t>
+  </si>
+  <si>
+    <t>tag_uc</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Census ID</t>
+  </si>
+  <si>
+    <t>Asset Index (PCA) (Post-Quake)</t>
+  </si>
+  <si>
+    <t>Asset Index (PCA) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Total Annual Food Expenditure</t>
+  </si>
+  <si>
+    <t>Total Annual Nonfood Expenditure</t>
+  </si>
+  <si>
+    <t>Eligible for death compensation?</t>
+  </si>
+  <si>
+    <t>District Code</t>
+  </si>
+  <si>
+    <t>District Abbottabad</t>
+  </si>
+  <si>
+    <t>District Bagh</t>
+  </si>
+  <si>
+    <t>District Mansehra</t>
+  </si>
+  <si>
+    <t>District Muzaffarabad</t>
+  </si>
+  <si>
+    <t>Distance to Epicenter (km)</t>
+  </si>
+  <si>
+    <t>Family Size</t>
+  </si>
+  <si>
+    <t>Closest Faultline (km)</t>
+  </si>
+  <si>
+    <t>Distance to Faultline (km)</t>
+  </si>
+  <si>
+    <t>Amount received from housing compensation</t>
+  </si>
+  <si>
+    <t>Eligible for housing compensation?</t>
+  </si>
+  <si>
+    <t>Did any member receive 1st trench of 25,000 rupee grant immediately following EQ</t>
+  </si>
+  <si>
+    <t>Eligible for injury compensation?</t>
+  </si>
+  <si>
+    <t>Eligible for lcgs compensation?</t>
+  </si>
+  <si>
+    <t>Mean Slope of UC</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Gov't School (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Log Dist to Distr Office (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Gov't School (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Market (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Medical (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Private School (min)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Market (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Medical Facility (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Private School (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Distance to Water (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Village Code</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Financial</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Health and Medical</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Shelter</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Food</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Supplies</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Liaison with other organizations</t>
+  </si>
+  <si>
+    <t>Above Median Elevation</t>
+  </si>
+  <si>
+    <t>Distance to Water (km)</t>
+  </si>
+  <si>
+    <t>Distance to Health Clinic (km)</t>
+  </si>
+  <si>
+    <t>Distance to Boys School (km)</t>
+  </si>
+  <si>
+    <t>Distance to Girls School (km)</t>
+  </si>
+  <si>
+    <t>Distance to Private School (km)</t>
+  </si>
+  <si>
+    <t>Far from Fault (&gt;20km)</t>
+  </si>
+  <si>
+    <t>Permanent House (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Total Reported Aid Compensation</t>
+  </si>
+  <si>
+    <t>Number Dead in Earthquake</t>
+  </si>
+  <si>
+    <t>(log) Consumption per Capita</t>
+  </si>
+  <si>
+    <t>Beds/Charpais</t>
+  </si>
+  <si>
+    <t>Tables</t>
+  </si>
+  <si>
+    <t>Chairs</t>
+  </si>
+  <si>
+    <t>Fans (Ceiling/Table/Pedestal/Exhaust)</t>
+  </si>
+  <si>
+    <t>Sewing machine</t>
+  </si>
+  <si>
+    <t>Books</t>
+  </si>
+  <si>
+    <t>Refrigerator</t>
+  </si>
+  <si>
+    <t>Radio/Cassette recorder/CD Player</t>
+  </si>
+  <si>
+    <t>Television</t>
+  </si>
+  <si>
+    <t>VCR/VCD</t>
+  </si>
+  <si>
+    <t>Watches</t>
+  </si>
+  <si>
+    <t>Guns</t>
+  </si>
+  <si>
+    <t>Plough</t>
+  </si>
+  <si>
+    <t>Tractor</t>
+  </si>
+  <si>
+    <t>Tube well/Hand pump</t>
+  </si>
+  <si>
+    <t>Other Agricultural Machinery</t>
+  </si>
+  <si>
+    <t>Other Agricultural Hand-Tools/Saw</t>
+  </si>
+  <si>
+    <t>Motorcycle/Scooter</t>
+  </si>
+  <si>
+    <t>Car/Taxi/Vehicle</t>
+  </si>
+  <si>
+    <t>Bicycle</t>
+  </si>
+  <si>
+    <t>Cattle</t>
+  </si>
+  <si>
+    <t>Goats</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Mobile Phone</t>
+  </si>
+  <si>
+    <t>Water In House (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Water In House (Post-Quake)</t>
+  </si>
+  <si>
+    <t>Household Infrastructure Index</t>
+  </si>
+  <si>
+    <t>Union Council Tag</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>choices</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>catyes</t>
+  </si>
+  <si>
+    <t>hh_elevation_binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>perm</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>dead_l</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t>perm</t>
+  </si>
+  <si>
+    <t>catyes</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Non-permanent Housing</t>
+  </si>
+  <si>
+    <t>Permanent Housing</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Don't Know</t>
+  </si>
+  <si>
+    <t>Neelum</t>
+  </si>
+  <si>
+    <t>Abbotabad</t>
+  </si>
+  <si>
+    <t>Bagh</t>
+  </si>
+  <si>
+    <t>Mansehra</t>
+  </si>
+  <si>
+    <t>Muzaffarabad</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>censusid</t>
+  </si>
+  <si>
+    <t>hh_assets_pca_post</t>
+  </si>
+  <si>
+    <t>hh_assets_pca_pre</t>
+  </si>
+  <si>
+    <t>hh_consumption_food</t>
+  </si>
+  <si>
+    <t>hh_consumption_nonfood</t>
+  </si>
+  <si>
+    <t>hh_death_eligible</t>
+  </si>
+  <si>
+    <t>hh_district</t>
+  </si>
+  <si>
+    <t>hh_district_1</t>
+  </si>
+  <si>
+    <t>hh_district_2</t>
+  </si>
+  <si>
+    <t>hh_district_3</t>
+  </si>
+  <si>
+    <t>hh_district_4</t>
+  </si>
+  <si>
+    <t>hh_epidist</t>
+  </si>
+  <si>
+    <t>hh_familysize</t>
+  </si>
+  <si>
+    <t>hh_fault_minimum</t>
+  </si>
+  <si>
+    <t>hh_faultdist</t>
+  </si>
+  <si>
+    <t>hh_housing_amount</t>
+  </si>
+  <si>
+    <t>hh_housing_eligible</t>
+  </si>
+  <si>
+    <t>hh_housing_mSec16_q1_trench1</t>
+  </si>
+  <si>
+    <t>hh_injury_eligible</t>
+  </si>
+  <si>
+    <t>hh_lcgs_eligible</t>
+  </si>
+  <si>
+    <t>hh_slope</t>
+  </si>
+  <si>
+    <t>hh_stats_electricity_post</t>
+  </si>
+  <si>
+    <t>hh_stats_electricity_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_govtschool_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_logdistrict_post</t>
+  </si>
+  <si>
+    <t>hh_stats_loggschool_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logmarket_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logmedical_post</t>
+  </si>
+  <si>
+    <t>hh_stats_logprischool_post</t>
+  </si>
+  <si>
+    <t>hh_stats_market_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_medical_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_privateschool_pre</t>
+  </si>
+  <si>
+    <t>hh_stats_water_dist_pre</t>
+  </si>
+  <si>
+    <t>village_code</t>
+  </si>
+  <si>
+    <t>hh_aid_any_1</t>
+  </si>
+  <si>
+    <t>hh_aid_any_2</t>
+  </si>
+  <si>
+    <t>hh_aid_any_3</t>
+  </si>
+  <si>
+    <t>hh_aid_any_4</t>
+  </si>
+  <si>
+    <t>hh_aid_any_5</t>
+  </si>
+  <si>
+    <t>hh_aid_any_6</t>
+  </si>
+  <si>
+    <t>hh_elevation_binary</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_1</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_2</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_4</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_5</t>
+  </si>
+  <si>
+    <t>hh_distance_pre_6</t>
+  </si>
+  <si>
+    <t>hh_far_from_quake</t>
+  </si>
+  <si>
+    <t>hh_perm_house_pre</t>
+  </si>
+  <si>
+    <t>hh_perm_house_post</t>
+  </si>
+  <si>
+    <t>hh_aid_total</t>
+  </si>
+  <si>
+    <t>hh_dead</t>
+  </si>
+  <si>
+    <t>hh_logconscap</t>
+  </si>
+  <si>
+    <t>hh_assets_1_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_2_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_3_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_4_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_5_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_6_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_7_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_8_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_9_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_10_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_11_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_12_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_13_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_14_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_15_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_16_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_17_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_18_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_19_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_20_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_21_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_22_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_23_pre</t>
+  </si>
+  <si>
+    <t>hh_assets_24_pre</t>
+  </si>
+  <si>
+    <t>hh_water_inhouse_pre</t>
+  </si>
+  <si>
+    <t>hh_water_inhouse_post</t>
+  </si>
+  <si>
+    <t>hh_infra_index_post</t>
+  </si>
+  <si>
+    <t>tag_uc</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Census ID</t>
+  </si>
+  <si>
+    <t>Asset Index (PCA) (Post-Quake)</t>
+  </si>
+  <si>
+    <t>Asset Index (PCA) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Total Annual Food Expenditure</t>
+  </si>
+  <si>
+    <t>Total Annual Nonfood Expenditure</t>
+  </si>
+  <si>
+    <t>Eligible for death compensation?</t>
+  </si>
+  <si>
+    <t>District Code</t>
+  </si>
+  <si>
+    <t>District Abbottabad</t>
+  </si>
+  <si>
+    <t>District Bagh</t>
+  </si>
+  <si>
+    <t>District Mansehra</t>
+  </si>
+  <si>
+    <t>District Muzaffarabad</t>
+  </si>
+  <si>
+    <t>Distance to Epicenter (km)</t>
+  </si>
+  <si>
+    <t>Family Size</t>
+  </si>
+  <si>
+    <t>Closest Faultline (km)</t>
+  </si>
+  <si>
+    <t>Distance to Faultline (km)</t>
+  </si>
+  <si>
+    <t>Amount received from housing compensation</t>
+  </si>
+  <si>
+    <t>Eligible for housing compensation?</t>
+  </si>
+  <si>
+    <t>Did any member receive 1st trench of 25,000 rupee grant immediately following EQ</t>
+  </si>
+  <si>
+    <t>Eligible for injury compensation?</t>
+  </si>
+  <si>
+    <t>Eligible for lcgs compensation?</t>
+  </si>
+  <si>
+    <t>Mean Slope of UC</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Gov't School (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Log Dist to Distr Office (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Gov't School (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Market (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Medical (min)</t>
+  </si>
+  <si>
+    <t>Log Dist to Private School (min)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Market (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Medical Facility (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Dist to Nearest Private School (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Distance to Water (min) (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Village Code</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Financial</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Health and Medical</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Shelter</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Food</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Supplies</t>
+  </si>
+  <si>
+    <t>Type of help (A) 1?: Any Liaison with other organizations</t>
+  </si>
+  <si>
+    <t>Above Median Elevation</t>
+  </si>
+  <si>
+    <t>Distance to Water (km)</t>
+  </si>
+  <si>
+    <t>Distance to Health Clinic (km)</t>
+  </si>
+  <si>
+    <t>Distance to Boys School (km)</t>
+  </si>
+  <si>
+    <t>Distance to Girls School (km)</t>
+  </si>
+  <si>
+    <t>Distance to Private School (km)</t>
+  </si>
+  <si>
+    <t>Far from Fault (&gt;20km)</t>
+  </si>
+  <si>
+    <t>Permanent House (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Total Reported Aid Compensation</t>
+  </si>
+  <si>
+    <t>Number Dead in Earthquake</t>
+  </si>
+  <si>
+    <t>(log) Consumption per Capita</t>
+  </si>
+  <si>
+    <t>Beds/Charpais</t>
+  </si>
+  <si>
+    <t>Tables</t>
+  </si>
+  <si>
+    <t>Chairs</t>
+  </si>
+  <si>
+    <t>Fans (Ceiling/Table/Pedestal/Exhaust)</t>
+  </si>
+  <si>
+    <t>Sewing machine</t>
+  </si>
+  <si>
+    <t>Books</t>
+  </si>
+  <si>
+    <t>Refrigerator</t>
+  </si>
+  <si>
+    <t>Radio/Cassette recorder/CD Player</t>
+  </si>
+  <si>
+    <t>Television</t>
+  </si>
+  <si>
+    <t>VCR/VCD</t>
+  </si>
+  <si>
+    <t>Watches</t>
+  </si>
+  <si>
+    <t>Guns</t>
+  </si>
+  <si>
+    <t>Plough</t>
+  </si>
+  <si>
+    <t>Tractor</t>
+  </si>
+  <si>
+    <t>Tube well/Hand pump</t>
+  </si>
+  <si>
+    <t>Other Agricultural Machinery</t>
+  </si>
+  <si>
+    <t>Other Agricultural Hand-Tools/Saw</t>
+  </si>
+  <si>
+    <t>Motorcycle/Scooter</t>
+  </si>
+  <si>
+    <t>Car/Taxi/Vehicle</t>
+  </si>
+  <si>
+    <t>Bicycle</t>
+  </si>
+  <si>
+    <t>Cattle</t>
+  </si>
+  <si>
+    <t>Goats</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Mobile Phone</t>
+  </si>
+  <si>
+    <t>Water In House (Pre-Quake)</t>
+  </si>
+  <si>
+    <t>Water In House (Post-Quake)</t>
+  </si>
+  <si>
+    <t>Household Infrastructure Index</t>
+  </si>
+  <si>
+    <t>Union Council Tag</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>choices</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>catyes</t>
+  </si>
+  <si>
+    <t>hh_elevation_binary</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>perm</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>dead_l</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>yesno</t>
@@ -6245,1136 +7865,1136 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>1791</v>
+        <v>2331</v>
       </c>
       <c r="B1" t="s">
-        <v>1872</v>
+        <v>2412</v>
       </c>
       <c r="C1" t="s">
-        <v>1951</v>
+        <v>2491</v>
       </c>
       <c r="D1" t="s">
-        <v>1976</v>
+        <v>2516</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1792</v>
+        <v>2332</v>
       </c>
       <c r="B2" t="s">
-        <v>1873</v>
+        <v>2413</v>
       </c>
       <c r="C2" t="s">
-        <v>1952</v>
+        <v>2492</v>
       </c>
       <c r="D2" t="s">
-        <v>1977</v>
+        <v>2517</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>1793</v>
+        <v>2333</v>
       </c>
       <c r="B3" t="s">
-        <v>1874</v>
+        <v>2414</v>
       </c>
       <c r="C3" t="s">
-        <v>1953</v>
+        <v>2493</v>
       </c>
       <c r="D3" t="s">
-        <v>1978</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>1794</v>
+        <v>2334</v>
       </c>
       <c r="B4" t="s">
-        <v>1875</v>
+        <v>2415</v>
       </c>
       <c r="C4" t="s">
-        <v>1953</v>
+        <v>2493</v>
       </c>
       <c r="D4" t="s">
-        <v>1979</v>
+        <v>2519</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>1795</v>
+        <v>2335</v>
       </c>
       <c r="B5" t="s">
-        <v>1876</v>
+        <v>2416</v>
       </c>
       <c r="C5" t="s">
-        <v>1953</v>
+        <v>2493</v>
       </c>
       <c r="D5" t="s">
-        <v>1980</v>
+        <v>2520</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>1796</v>
+        <v>2336</v>
       </c>
       <c r="B6" t="s">
-        <v>1877</v>
+        <v>2417</v>
       </c>
       <c r="C6" t="s">
-        <v>1953</v>
+        <v>2493</v>
       </c>
       <c r="D6" t="s">
-        <v>1981</v>
+        <v>2521</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>1797</v>
+        <v>2337</v>
       </c>
       <c r="B7" t="s">
-        <v>1878</v>
+        <v>2418</v>
       </c>
       <c r="C7" t="s">
-        <v>1954</v>
+        <v>2494</v>
       </c>
       <c r="D7" t="s">
-        <v>1982</v>
+        <v>2522</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>1798</v>
+        <v>2338</v>
       </c>
       <c r="B8" t="s">
-        <v>1879</v>
+        <v>2419</v>
       </c>
       <c r="C8" t="s">
-        <v>1954</v>
+        <v>2494</v>
       </c>
       <c r="D8" t="s">
-        <v>1983</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>1799</v>
+        <v>2339</v>
       </c>
       <c r="B9" t="s">
-        <v>1880</v>
+        <v>2420</v>
       </c>
       <c r="C9" t="s">
-        <v>1954</v>
+        <v>2494</v>
       </c>
       <c r="D9" t="s">
-        <v>1984</v>
+        <v>2524</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>1800</v>
+        <v>2340</v>
       </c>
       <c r="B10" t="s">
-        <v>1881</v>
+        <v>2421</v>
       </c>
       <c r="C10" t="s">
-        <v>1954</v>
+        <v>2494</v>
       </c>
       <c r="D10" t="s">
-        <v>1985</v>
+        <v>2525</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>1801</v>
+        <v>2341</v>
       </c>
       <c r="B11" t="s">
-        <v>1882</v>
+        <v>2422</v>
       </c>
       <c r="C11" t="s">
-        <v>1954</v>
+        <v>2494</v>
       </c>
       <c r="D11" t="s">
-        <v>1986</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>1802</v>
+        <v>2342</v>
       </c>
       <c r="B12" t="s">
-        <v>1883</v>
+        <v>2423</v>
       </c>
       <c r="C12" t="s">
-        <v>1954</v>
+        <v>2494</v>
       </c>
       <c r="D12" t="s">
-        <v>1987</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>1803</v>
+        <v>2343</v>
       </c>
       <c r="B13" t="s">
-        <v>1884</v>
+        <v>2424</v>
       </c>
       <c r="C13" t="s">
-        <v>1955</v>
+        <v>2495</v>
       </c>
       <c r="D13" t="s">
-        <v>1988</v>
+        <v>2528</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>1804</v>
+        <v>2344</v>
       </c>
       <c r="B14" t="s">
-        <v>1885</v>
+        <v>2425</v>
       </c>
       <c r="C14" t="s">
-        <v>1956</v>
+        <v>2496</v>
       </c>
       <c r="D14" t="s">
-        <v>1989</v>
+        <v>2529</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>1805</v>
+        <v>2345</v>
       </c>
       <c r="B15" t="s">
-        <v>1886</v>
+        <v>2426</v>
       </c>
       <c r="C15" t="s">
-        <v>1957</v>
+        <v>2497</v>
       </c>
       <c r="D15" t="s">
-        <v>1990</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>1806</v>
+        <v>2346</v>
       </c>
       <c r="B16" t="s">
-        <v>1887</v>
+        <v>2427</v>
       </c>
       <c r="C16" t="s">
-        <v>1957</v>
+        <v>2497</v>
       </c>
       <c r="D16" t="s">
-        <v>1991</v>
+        <v>2531</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>1807</v>
+        <v>2347</v>
       </c>
       <c r="B17" t="s">
-        <v>1888</v>
+        <v>2428</v>
       </c>
       <c r="C17" t="s">
-        <v>1958</v>
+        <v>2498</v>
       </c>
       <c r="D17" t="s">
-        <v>1992</v>
+        <v>2532</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>1808</v>
+        <v>2348</v>
       </c>
       <c r="B18" t="s">
-        <v>1889</v>
+        <v>2429</v>
       </c>
       <c r="C18" t="s">
-        <v>1959</v>
+        <v>2499</v>
       </c>
       <c r="D18" t="s">
-        <v>1993</v>
+        <v>2533</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>1809</v>
+        <v>2349</v>
       </c>
       <c r="B19" t="s">
-        <v>1890</v>
+        <v>2430</v>
       </c>
       <c r="C19" t="s">
-        <v>1959</v>
+        <v>2499</v>
       </c>
       <c r="D19" t="s">
-        <v>1993</v>
+        <v>2533</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>1810</v>
+        <v>2350</v>
       </c>
       <c r="B20" t="s">
-        <v>1891</v>
+        <v>2431</v>
       </c>
       <c r="C20" t="s">
-        <v>1959</v>
+        <v>2499</v>
       </c>
       <c r="D20" t="s">
-        <v>1993</v>
+        <v>2533</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>1811</v>
+        <v>2351</v>
       </c>
       <c r="B21" t="s">
-        <v>1892</v>
+        <v>2432</v>
       </c>
       <c r="C21" t="s">
-        <v>1959</v>
+        <v>2499</v>
       </c>
       <c r="D21" t="s">
-        <v>1993</v>
+        <v>2533</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>1812</v>
+        <v>2352</v>
       </c>
       <c r="B22" t="s">
-        <v>1893</v>
+        <v>2433</v>
       </c>
       <c r="C22" t="s">
-        <v>1960</v>
+        <v>2500</v>
       </c>
       <c r="D22" t="s">
-        <v>1994</v>
+        <v>2534</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>1813</v>
+        <v>2353</v>
       </c>
       <c r="B23" t="s">
-        <v>1894</v>
+        <v>2434</v>
       </c>
       <c r="C23" t="s">
-        <v>1961</v>
+        <v>2501</v>
       </c>
       <c r="D23" t="s">
-        <v>1995</v>
+        <v>2535</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>1814</v>
+        <v>2354</v>
       </c>
       <c r="B24" t="s">
-        <v>1894</v>
+        <v>2434</v>
       </c>
       <c r="C24" t="s">
-        <v>1961</v>
+        <v>2501</v>
       </c>
       <c r="D24" t="s">
-        <v>1995</v>
+        <v>2535</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>1815</v>
+        <v>2355</v>
       </c>
       <c r="B25" t="s">
-        <v>1895</v>
+        <v>2435</v>
       </c>
       <c r="C25" t="s">
-        <v>1962</v>
+        <v>2502</v>
       </c>
       <c r="D25" t="s">
-        <v>1996</v>
+        <v>2536</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>1816</v>
+        <v>2356</v>
       </c>
       <c r="B26" t="s">
-        <v>1896</v>
+        <v>2436</v>
       </c>
       <c r="C26" t="s">
-        <v>1963</v>
+        <v>2503</v>
       </c>
       <c r="D26" t="s">
-        <v>1997</v>
+        <v>2537</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>1817</v>
+        <v>2357</v>
       </c>
       <c r="B27" t="s">
-        <v>1897</v>
+        <v>2437</v>
       </c>
       <c r="C27" t="s">
-        <v>1963</v>
+        <v>2503</v>
       </c>
       <c r="D27" t="s">
-        <v>1998</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>1818</v>
+        <v>2358</v>
       </c>
       <c r="B28" t="s">
-        <v>1898</v>
+        <v>2438</v>
       </c>
       <c r="C28" t="s">
-        <v>1963</v>
+        <v>2503</v>
       </c>
       <c r="D28" t="s">
-        <v>1999</v>
+        <v>2539</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>1819</v>
+        <v>2359</v>
       </c>
       <c r="B29" t="s">
-        <v>1899</v>
+        <v>2439</v>
       </c>
       <c r="C29" t="s">
-        <v>1963</v>
+        <v>2503</v>
       </c>
       <c r="D29" t="s">
-        <v>2000</v>
+        <v>2540</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>1820</v>
+        <v>2360</v>
       </c>
       <c r="B30" t="s">
-        <v>1900</v>
+        <v>2440</v>
       </c>
       <c r="C30" t="s">
-        <v>1963</v>
+        <v>2503</v>
       </c>
       <c r="D30" t="s">
-        <v>2001</v>
+        <v>2541</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>1821</v>
+        <v>2361</v>
       </c>
       <c r="B31" t="s">
-        <v>1901</v>
+        <v>2441</v>
       </c>
       <c r="C31" t="s">
-        <v>1964</v>
+        <v>2504</v>
       </c>
       <c r="D31" t="s">
-        <v>2002</v>
+        <v>2542</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>1822</v>
+        <v>2362</v>
       </c>
       <c r="B32" t="s">
-        <v>1902</v>
+        <v>2442</v>
       </c>
       <c r="C32" t="s">
-        <v>1964</v>
+        <v>2504</v>
       </c>
       <c r="D32" t="s">
-        <v>2003</v>
+        <v>2543</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>1823</v>
+        <v>2363</v>
       </c>
       <c r="B33" t="s">
-        <v>1903</v>
+        <v>2443</v>
       </c>
       <c r="C33" t="s">
-        <v>1964</v>
+        <v>2504</v>
       </c>
       <c r="D33" t="s">
-        <v>2004</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>1824</v>
+        <v>2364</v>
       </c>
       <c r="B34" t="s">
-        <v>1904</v>
+        <v>2444</v>
       </c>
       <c r="C34" t="s">
-        <v>1965</v>
+        <v>2505</v>
       </c>
       <c r="D34" t="s">
-        <v>2005</v>
+        <v>2545</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>1825</v>
+        <v>2365</v>
       </c>
       <c r="B35" t="s">
-        <v>1905</v>
+        <v>2445</v>
       </c>
       <c r="C35" t="s">
-        <v>1966</v>
+        <v>2506</v>
       </c>
       <c r="D35" t="s">
-        <v>2006</v>
+        <v>2546</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>1826</v>
+        <v>2366</v>
       </c>
       <c r="B36" t="s">
-        <v>1906</v>
+        <v>2446</v>
       </c>
       <c r="C36" t="s">
-        <v>1967</v>
+        <v>2507</v>
       </c>
       <c r="D36" t="s">
-        <v>2007</v>
+        <v>2547</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>1827</v>
+        <v>2367</v>
       </c>
       <c r="B37" t="s">
-        <v>1907</v>
+        <v>2447</v>
       </c>
       <c r="C37" t="s">
-        <v>1967</v>
+        <v>2507</v>
       </c>
       <c r="D37" t="s">
-        <v>2007</v>
+        <v>2547</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>1828</v>
+        <v>2368</v>
       </c>
       <c r="B38" t="s">
-        <v>1908</v>
+        <v>2448</v>
       </c>
       <c r="C38" t="s">
-        <v>1967</v>
+        <v>2507</v>
       </c>
       <c r="D38" t="s">
-        <v>2007</v>
+        <v>2547</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>1829</v>
+        <v>2369</v>
       </c>
       <c r="B39" t="s">
-        <v>1909</v>
+        <v>2449</v>
       </c>
       <c r="C39" t="s">
-        <v>1967</v>
+        <v>2507</v>
       </c>
       <c r="D39" t="s">
-        <v>2007</v>
+        <v>2547</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>1830</v>
+        <v>2370</v>
       </c>
       <c r="B40" t="s">
-        <v>1910</v>
+        <v>2450</v>
       </c>
       <c r="C40" t="s">
-        <v>1967</v>
+        <v>2507</v>
       </c>
       <c r="D40" t="s">
-        <v>2007</v>
+        <v>2547</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>1831</v>
+        <v>2371</v>
       </c>
       <c r="B41" t="s">
-        <v>1911</v>
+        <v>2451</v>
       </c>
       <c r="C41" t="s">
-        <v>1967</v>
+        <v>2507</v>
       </c>
       <c r="D41" t="s">
-        <v>2007</v>
+        <v>2547</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>1832</v>
+        <v>2372</v>
       </c>
       <c r="B42" t="s">
-        <v>1912</v>
+        <v>2452</v>
       </c>
       <c r="C42" t="s">
-        <v>1967</v>
+        <v>2507</v>
       </c>
       <c r="D42" t="s">
-        <v>2008</v>
+        <v>2548</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>1833</v>
+        <v>2373</v>
       </c>
       <c r="B43" t="s">
-        <v>1913</v>
+        <v>2453</v>
       </c>
       <c r="C43" t="s">
-        <v>1968</v>
+        <v>2508</v>
       </c>
       <c r="D43" t="s">
-        <v>2009</v>
+        <v>2549</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>1834</v>
+        <v>2374</v>
       </c>
       <c r="B44" t="s">
-        <v>1914</v>
+        <v>2454</v>
       </c>
       <c r="C44" t="s">
-        <v>1968</v>
+        <v>2508</v>
       </c>
       <c r="D44" t="s">
-        <v>2010</v>
+        <v>2550</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>1835</v>
+        <v>2375</v>
       </c>
       <c r="B45" t="s">
-        <v>1915</v>
+        <v>2455</v>
       </c>
       <c r="C45" t="s">
-        <v>1968</v>
+        <v>2508</v>
       </c>
       <c r="D45" t="s">
-        <v>2011</v>
+        <v>2551</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>1836</v>
+        <v>2376</v>
       </c>
       <c r="B46" t="s">
-        <v>1916</v>
+        <v>2456</v>
       </c>
       <c r="C46" t="s">
-        <v>1968</v>
+        <v>2508</v>
       </c>
       <c r="D46" t="s">
-        <v>2012</v>
+        <v>2552</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>1837</v>
+        <v>2377</v>
       </c>
       <c r="B47" t="s">
-        <v>1917</v>
+        <v>2457</v>
       </c>
       <c r="C47" t="s">
-        <v>1968</v>
+        <v>2508</v>
       </c>
       <c r="D47" t="s">
-        <v>2013</v>
+        <v>2553</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>1838</v>
+        <v>2378</v>
       </c>
       <c r="B48" t="s">
-        <v>1918</v>
+        <v>2458</v>
       </c>
       <c r="C48" t="s">
-        <v>1969</v>
+        <v>2509</v>
       </c>
       <c r="D48" t="s">
-        <v>2014</v>
+        <v>2554</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>1839</v>
+        <v>2379</v>
       </c>
       <c r="B49" t="s">
-        <v>1919</v>
+        <v>2459</v>
       </c>
       <c r="C49" t="s">
-        <v>1969</v>
+        <v>2509</v>
       </c>
       <c r="D49" t="s">
-        <v>2015</v>
+        <v>2555</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>1840</v>
+        <v>2380</v>
       </c>
       <c r="B50" t="s">
-        <v>1919</v>
+        <v>2459</v>
       </c>
       <c r="C50" t="s">
-        <v>1969</v>
+        <v>2509</v>
       </c>
       <c r="D50" t="s">
-        <v>2016</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>1841</v>
+        <v>2381</v>
       </c>
       <c r="B51" t="s">
-        <v>1920</v>
+        <v>2460</v>
       </c>
       <c r="C51" t="s">
-        <v>1970</v>
+        <v>2510</v>
       </c>
       <c r="D51" t="s">
-        <v>2017</v>
+        <v>2557</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>1842</v>
+        <v>2382</v>
       </c>
       <c r="B52" t="s">
-        <v>1921</v>
+        <v>2461</v>
       </c>
       <c r="C52" t="s">
-        <v>1971</v>
+        <v>2511</v>
       </c>
       <c r="D52" t="s">
-        <v>2018</v>
+        <v>2558</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>1843</v>
+        <v>2383</v>
       </c>
       <c r="B53" t="s">
-        <v>1922</v>
+        <v>2462</v>
       </c>
       <c r="C53" t="s">
-        <v>1972</v>
+        <v>2512</v>
       </c>
       <c r="D53" t="s">
-        <v>2019</v>
+        <v>2559</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>1844</v>
+        <v>2384</v>
       </c>
       <c r="B54" t="s">
-        <v>1923</v>
+        <v>2463</v>
       </c>
       <c r="C54" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D54" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>1845</v>
+        <v>2385</v>
       </c>
       <c r="B55" t="s">
-        <v>1924</v>
+        <v>2464</v>
       </c>
       <c r="C55" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D55" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>1846</v>
+        <v>2386</v>
       </c>
       <c r="B56" t="s">
-        <v>1925</v>
+        <v>2465</v>
       </c>
       <c r="C56" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D56" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>1847</v>
+        <v>2387</v>
       </c>
       <c r="B57" t="s">
-        <v>1926</v>
+        <v>2466</v>
       </c>
       <c r="C57" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D57" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>1848</v>
+        <v>2388</v>
       </c>
       <c r="B58" t="s">
-        <v>1927</v>
+        <v>2467</v>
       </c>
       <c r="C58" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D58" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>1849</v>
+        <v>2389</v>
       </c>
       <c r="B59" t="s">
-        <v>1928</v>
+        <v>2468</v>
       </c>
       <c r="C59" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D59" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>1850</v>
+        <v>2390</v>
       </c>
       <c r="B60" t="s">
-        <v>1929</v>
+        <v>2469</v>
       </c>
       <c r="C60" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D60" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>1851</v>
+        <v>2391</v>
       </c>
       <c r="B61" t="s">
-        <v>1930</v>
+        <v>2470</v>
       </c>
       <c r="C61" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D61" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>1852</v>
+        <v>2392</v>
       </c>
       <c r="B62" t="s">
-        <v>1931</v>
+        <v>2471</v>
       </c>
       <c r="C62" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D62" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>1853</v>
+        <v>2393</v>
       </c>
       <c r="B63" t="s">
-        <v>1932</v>
+        <v>2472</v>
       </c>
       <c r="C63" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D63" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>1854</v>
+        <v>2394</v>
       </c>
       <c r="B64" t="s">
-        <v>1933</v>
+        <v>2473</v>
       </c>
       <c r="C64" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D64" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>1855</v>
+        <v>2395</v>
       </c>
       <c r="B65" t="s">
-        <v>1934</v>
+        <v>2474</v>
       </c>
       <c r="C65" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D65" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>1856</v>
+        <v>2396</v>
       </c>
       <c r="B66" t="s">
-        <v>1935</v>
+        <v>2475</v>
       </c>
       <c r="C66" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D66" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>1857</v>
+        <v>2397</v>
       </c>
       <c r="B67" t="s">
-        <v>1936</v>
+        <v>2476</v>
       </c>
       <c r="C67" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D67" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>1858</v>
+        <v>2398</v>
       </c>
       <c r="B68" t="s">
-        <v>1937</v>
+        <v>2477</v>
       </c>
       <c r="C68" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D68" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>1859</v>
+        <v>2399</v>
       </c>
       <c r="B69" t="s">
-        <v>1938</v>
+        <v>2478</v>
       </c>
       <c r="C69" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D69" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>1860</v>
+        <v>2400</v>
       </c>
       <c r="B70" t="s">
-        <v>1939</v>
+        <v>2479</v>
       </c>
       <c r="C70" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D70" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>1861</v>
+        <v>2401</v>
       </c>
       <c r="B71" t="s">
-        <v>1940</v>
+        <v>2480</v>
       </c>
       <c r="C71" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D71" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>1862</v>
+        <v>2402</v>
       </c>
       <c r="B72" t="s">
-        <v>1941</v>
+        <v>2481</v>
       </c>
       <c r="C72" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D72" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>1863</v>
+        <v>2403</v>
       </c>
       <c r="B73" t="s">
-        <v>1942</v>
+        <v>2482</v>
       </c>
       <c r="C73" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D73" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>1864</v>
+        <v>2404</v>
       </c>
       <c r="B74" t="s">
-        <v>1943</v>
+        <v>2483</v>
       </c>
       <c r="C74" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D74" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>1865</v>
+        <v>2405</v>
       </c>
       <c r="B75" t="s">
-        <v>1944</v>
+        <v>2484</v>
       </c>
       <c r="C75" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D75" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>1866</v>
+        <v>2406</v>
       </c>
       <c r="B76" t="s">
-        <v>1945</v>
+        <v>2485</v>
       </c>
       <c r="C76" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D76" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>1867</v>
+        <v>2407</v>
       </c>
       <c r="B77" t="s">
-        <v>1946</v>
+        <v>2486</v>
       </c>
       <c r="C77" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D77" t="s">
-        <v>2020</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>1868</v>
+        <v>2408</v>
       </c>
       <c r="B78" t="s">
-        <v>1947</v>
+        <v>2487</v>
       </c>
       <c r="C78" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D78" t="s">
-        <v>2021</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>1869</v>
+        <v>2409</v>
       </c>
       <c r="B79" t="s">
-        <v>1948</v>
+        <v>2488</v>
       </c>
       <c r="C79" t="s">
-        <v>1973</v>
+        <v>2513</v>
       </c>
       <c r="D79" t="s">
-        <v>2022</v>
+        <v>2562</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>1870</v>
+        <v>2410</v>
       </c>
       <c r="B80" t="s">
-        <v>1949</v>
+        <v>2489</v>
       </c>
       <c r="C80" t="s">
-        <v>1974</v>
+        <v>2514</v>
       </c>
       <c r="D80" t="s">
-        <v>2023</v>
+        <v>2563</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>1871</v>
+        <v>2411</v>
       </c>
       <c r="B81" t="s">
-        <v>1950</v>
+        <v>2490</v>
       </c>
       <c r="C81" t="s">
-        <v>1975</v>
+        <v>2515</v>
       </c>
       <c r="D81" t="s">
-        <v>2024</v>
+        <v>2564</v>
       </c>
     </row>
   </sheetData>
@@ -7388,167 +9008,167 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>2025</v>
+        <v>2565</v>
       </c>
       <c r="B1" t="s">
-        <v>2031</v>
+        <v>2571</v>
       </c>
       <c r="C1" t="s">
-        <v>2046</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2026</v>
+        <v>2566</v>
       </c>
       <c r="B2" t="s">
-        <v>2032</v>
+        <v>2572</v>
       </c>
       <c r="C2" t="s">
-        <v>2047</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2026</v>
+        <v>2566</v>
       </c>
       <c r="B3" t="s">
-        <v>2033</v>
+        <v>2573</v>
       </c>
       <c r="C3" t="s">
-        <v>2048</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2027</v>
+        <v>2567</v>
       </c>
       <c r="B4" t="s">
-        <v>2034</v>
+        <v>2574</v>
       </c>
       <c r="C4" t="s">
-        <v>2049</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2027</v>
+        <v>2567</v>
       </c>
       <c r="B5" t="s">
-        <v>2035</v>
+        <v>2575</v>
       </c>
       <c r="C5" t="s">
-        <v>2050</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>2028</v>
+        <v>2568</v>
       </c>
       <c r="B6" t="s">
-        <v>2036</v>
+        <v>2576</v>
       </c>
       <c r="C6" t="s">
-        <v>2051</v>
+        <v>2591</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2028</v>
+        <v>2568</v>
       </c>
       <c r="B7" t="s">
-        <v>2037</v>
+        <v>2577</v>
       </c>
       <c r="C7" t="s">
-        <v>2052</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>2029</v>
+        <v>2569</v>
       </c>
       <c r="B8" t="s">
-        <v>2038</v>
+        <v>2578</v>
       </c>
       <c r="C8" t="s">
-        <v>2053</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>2029</v>
+        <v>2569</v>
       </c>
       <c r="B9" t="s">
-        <v>2039</v>
+        <v>2579</v>
       </c>
       <c r="C9" t="s">
-        <v>2054</v>
+        <v>2594</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>2029</v>
+        <v>2569</v>
       </c>
       <c r="B10" t="s">
-        <v>2040</v>
+        <v>2580</v>
       </c>
       <c r="C10" t="s">
-        <v>2055</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>2030</v>
+        <v>2570</v>
       </c>
       <c r="B11" t="s">
-        <v>2041</v>
+        <v>2581</v>
       </c>
       <c r="C11" t="s">
-        <v>2056</v>
+        <v>2596</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>2030</v>
+        <v>2570</v>
       </c>
       <c r="B12" t="s">
-        <v>2042</v>
+        <v>2582</v>
       </c>
       <c r="C12" t="s">
-        <v>2057</v>
+        <v>2597</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>2030</v>
+        <v>2570</v>
       </c>
       <c r="B13" t="s">
-        <v>2043</v>
+        <v>2583</v>
       </c>
       <c r="C13" t="s">
-        <v>2058</v>
+        <v>2598</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>2030</v>
+        <v>2570</v>
       </c>
       <c r="B14" t="s">
-        <v>2044</v>
+        <v>2584</v>
       </c>
       <c r="C14" t="s">
-        <v>2059</v>
+        <v>2599</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>2030</v>
+        <v>2570</v>
       </c>
       <c r="B15" t="s">
-        <v>2045</v>
+        <v>2585</v>
       </c>
       <c r="C15" t="s">
-        <v>2060</v>
+        <v>2600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>